<commit_message>
code jusqu'à max rsquared
</commit_message>
<xml_diff>
--- a/data/WVS7graphs.xlsx
+++ b/data/WVS7graphs.xlsx
@@ -8,196 +8,40 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julieta/Desktop/wellbeing_gdp_region/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E67584BC-7171-324E-B009-855C7DA9A34D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B0AC537-DCBA-6646-8951-990FFBD45394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="26960" windowHeight="15660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8760" yWindow="980" windowWidth="26960" windowHeight="15660" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="happiness_mean" sheetId="11" r:id="rId1"/>
     <sheet name="data" sheetId="1" r:id="rId2"/>
     <sheet name="satisfaction_mean" sheetId="7" r:id="rId3"/>
-    <sheet name="satisfied" sheetId="6" r:id="rId4"/>
-    <sheet name="ratio" sheetId="5" r:id="rId5"/>
-    <sheet name="very_unhappy" sheetId="4" r:id="rId6"/>
-    <sheet name="happy" sheetId="3" r:id="rId7"/>
-    <sheet name="very_happy" sheetId="2" r:id="rId8"/>
+    <sheet name="econometric results" sheetId="12" r:id="rId4"/>
+    <sheet name="satisfied" sheetId="6" r:id="rId5"/>
+    <sheet name="ratio" sheetId="5" r:id="rId6"/>
+    <sheet name="very_unhappy" sheetId="4" r:id="rId7"/>
+    <sheet name="happy" sheetId="3" r:id="rId8"/>
+    <sheet name="very_happy" sheetId="2" r:id="rId9"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">data!$A$2:$A$63</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">data!$B$2:$B$63</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">data!$G$1</definedName>
-    <definedName name="_xlchart.v1.100" hidden="1">data!$I$1</definedName>
-    <definedName name="_xlchart.v1.101" hidden="1">data!$I$2:$I$63</definedName>
-    <definedName name="_xlchart.v1.102" hidden="1">data!$J$1</definedName>
-    <definedName name="_xlchart.v1.103" hidden="1">data!$J$2:$J$63</definedName>
-    <definedName name="_xlchart.v1.104" hidden="1">data!$K$1</definedName>
-    <definedName name="_xlchart.v1.105" hidden="1">data!$K$2:$K$63</definedName>
-    <definedName name="_xlchart.v1.106" hidden="1">data!$A$2:$A$63</definedName>
-    <definedName name="_xlchart.v1.107" hidden="1">data!$B$2:$B$63</definedName>
-    <definedName name="_xlchart.v1.108" hidden="1">data!$C$1</definedName>
-    <definedName name="_xlchart.v1.109" hidden="1">data!$C$2:$C$63</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">data!$G$2:$G$63</definedName>
-    <definedName name="_xlchart.v1.110" hidden="1">data!$D$1</definedName>
-    <definedName name="_xlchart.v1.111" hidden="1">data!$D$2:$D$63</definedName>
-    <definedName name="_xlchart.v1.112" hidden="1">data!$E$1</definedName>
-    <definedName name="_xlchart.v1.113" hidden="1">data!$E$2:$E$63</definedName>
-    <definedName name="_xlchart.v1.114" hidden="1">data!$F$1</definedName>
-    <definedName name="_xlchart.v1.115" hidden="1">data!$F$2:$F$63</definedName>
-    <definedName name="_xlchart.v1.116" hidden="1">data!$G$1</definedName>
-    <definedName name="_xlchart.v1.117" hidden="1">data!$G$2:$G$63</definedName>
-    <definedName name="_xlchart.v1.118" hidden="1">data!$H$1</definedName>
-    <definedName name="_xlchart.v1.119" hidden="1">data!$H$2:$H$63</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">data!$H$1</definedName>
-    <definedName name="_xlchart.v1.120" hidden="1">data!$I$1</definedName>
-    <definedName name="_xlchart.v1.121" hidden="1">data!$I$2:$I$63</definedName>
-    <definedName name="_xlchart.v1.122" hidden="1">data!$J$1</definedName>
-    <definedName name="_xlchart.v1.123" hidden="1">data!$J$2:$J$63</definedName>
-    <definedName name="_xlchart.v1.124" hidden="1">data!$K$1</definedName>
-    <definedName name="_xlchart.v1.125" hidden="1">data!$K$2:$K$63</definedName>
-    <definedName name="_xlchart.v1.126" hidden="1">data!$B$2:$B$63</definedName>
-    <definedName name="_xlchart.v1.127" hidden="1">data!$E$2:$E$63</definedName>
-    <definedName name="_xlchart.v1.128" hidden="1">data!$A$2:$A$63</definedName>
-    <definedName name="_xlchart.v1.129" hidden="1">data!$B$2:$B$63</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">data!$H$2:$H$63</definedName>
-    <definedName name="_xlchart.v1.130" hidden="1">data!$C$1</definedName>
-    <definedName name="_xlchart.v1.131" hidden="1">data!$C$2:$C$63</definedName>
-    <definedName name="_xlchart.v1.132" hidden="1">data!$D$1</definedName>
-    <definedName name="_xlchart.v1.133" hidden="1">data!$D$2:$D$63</definedName>
-    <definedName name="_xlchart.v1.134" hidden="1">data!$E$1</definedName>
-    <definedName name="_xlchart.v1.135" hidden="1">data!$E$2:$E$63</definedName>
-    <definedName name="_xlchart.v1.136" hidden="1">data!$F$1</definedName>
-    <definedName name="_xlchart.v1.137" hidden="1">data!$F$2:$F$63</definedName>
-    <definedName name="_xlchart.v1.138" hidden="1">data!$G$1</definedName>
-    <definedName name="_xlchart.v1.139" hidden="1">data!$G$2:$G$63</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">data!$I$1</definedName>
-    <definedName name="_xlchart.v1.140" hidden="1">data!$H$1</definedName>
-    <definedName name="_xlchart.v1.141" hidden="1">data!$H$2:$H$63</definedName>
-    <definedName name="_xlchart.v1.142" hidden="1">data!$I$1</definedName>
-    <definedName name="_xlchart.v1.143" hidden="1">data!$I$2:$I$63</definedName>
-    <definedName name="_xlchart.v1.144" hidden="1">data!$J$1</definedName>
-    <definedName name="_xlchart.v1.145" hidden="1">data!$J$2:$J$63</definedName>
-    <definedName name="_xlchart.v1.146" hidden="1">data!$K$1</definedName>
-    <definedName name="_xlchart.v1.147" hidden="1">data!$K$2:$K$63</definedName>
-    <definedName name="_xlchart.v1.148" hidden="1">data!$A$2:$A$63</definedName>
-    <definedName name="_xlchart.v1.149" hidden="1">data!$B$2:$B$63</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">data!$I$2:$I$63</definedName>
-    <definedName name="_xlchart.v1.150" hidden="1">data!$C$1</definedName>
-    <definedName name="_xlchart.v1.151" hidden="1">data!$C$2:$C$63</definedName>
-    <definedName name="_xlchart.v1.152" hidden="1">data!$D$1</definedName>
-    <definedName name="_xlchart.v1.153" hidden="1">data!$D$2:$D$63</definedName>
-    <definedName name="_xlchart.v1.154" hidden="1">data!$E$1</definedName>
-    <definedName name="_xlchart.v1.155" hidden="1">data!$E$2:$E$63</definedName>
-    <definedName name="_xlchart.v1.156" hidden="1">data!$F$1</definedName>
-    <definedName name="_xlchart.v1.157" hidden="1">data!$F$2:$F$63</definedName>
-    <definedName name="_xlchart.v1.158" hidden="1">data!$G$1</definedName>
-    <definedName name="_xlchart.v1.159" hidden="1">data!$G$2:$G$63</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">data!$J$1</definedName>
-    <definedName name="_xlchart.v1.160" hidden="1">data!$H$1</definedName>
-    <definedName name="_xlchart.v1.161" hidden="1">data!$H$2:$H$63</definedName>
-    <definedName name="_xlchart.v1.162" hidden="1">data!$I$1</definedName>
-    <definedName name="_xlchart.v1.163" hidden="1">data!$I$2:$I$63</definedName>
-    <definedName name="_xlchart.v1.164" hidden="1">data!$J$1</definedName>
-    <definedName name="_xlchart.v1.165" hidden="1">data!$J$2:$J$63</definedName>
-    <definedName name="_xlchart.v1.166" hidden="1">data!$K$1</definedName>
-    <definedName name="_xlchart.v1.167" hidden="1">data!$K$2:$K$63</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">data!$J$2:$J$63</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">data!$K$1</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">data!$K$2:$K$63</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">data!$C$1</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">data!$A$2:$A$63</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">data!$B$1</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">data!$B$2:$B$63</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">data!$C$1</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">data!$C$2:$C$63</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">data!$D$1</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">data!$D$2:$D$63</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">data!$E$1</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">data!$E$2:$E$63</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">data!$F$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">data!$C$2:$C$63</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">data!$F$2:$F$63</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">data!$G$1</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">data!$G$2:$G$63</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">data!$H$1</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">data!$H$2:$H$63</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">data!$I$1</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">data!$I$2:$I$63</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">data!$J$1</definedName>
-    <definedName name="_xlchart.v1.38" hidden="1">data!$J$2:$J$63</definedName>
-    <definedName name="_xlchart.v1.39" hidden="1">data!$K$1</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">data!$D$1</definedName>
-    <definedName name="_xlchart.v1.40" hidden="1">data!$K$2:$K$63</definedName>
-    <definedName name="_xlchart.v1.41" hidden="1">data!$A$2:$A$63</definedName>
-    <definedName name="_xlchart.v1.42" hidden="1">data!$B$2:$B$63</definedName>
-    <definedName name="_xlchart.v1.43" hidden="1">data!$C$1</definedName>
-    <definedName name="_xlchart.v1.44" hidden="1">data!$C$2:$C$63</definedName>
-    <definedName name="_xlchart.v1.45" hidden="1">data!$D$1</definedName>
-    <definedName name="_xlchart.v1.46" hidden="1">data!$D$2:$D$63</definedName>
-    <definedName name="_xlchart.v1.47" hidden="1">data!$E$1</definedName>
-    <definedName name="_xlchart.v1.48" hidden="1">data!$E$2:$E$63</definedName>
-    <definedName name="_xlchart.v1.49" hidden="1">data!$F$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">data!$D$2:$D$63</definedName>
-    <definedName name="_xlchart.v1.50" hidden="1">data!$F$2:$F$63</definedName>
-    <definedName name="_xlchart.v1.51" hidden="1">data!$G$1</definedName>
-    <definedName name="_xlchart.v1.52" hidden="1">data!$G$2:$G$63</definedName>
-    <definedName name="_xlchart.v1.53" hidden="1">data!$H$1</definedName>
-    <definedName name="_xlchart.v1.54" hidden="1">data!$H$2:$H$63</definedName>
-    <definedName name="_xlchart.v1.55" hidden="1">data!$I$1</definedName>
-    <definedName name="_xlchart.v1.56" hidden="1">data!$I$2:$I$63</definedName>
-    <definedName name="_xlchart.v1.57" hidden="1">data!$J$1</definedName>
-    <definedName name="_xlchart.v1.58" hidden="1">data!$J$2:$J$63</definedName>
-    <definedName name="_xlchart.v1.59" hidden="1">data!$K$1</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">data!$E$1</definedName>
-    <definedName name="_xlchart.v1.60" hidden="1">data!$K$2:$K$63</definedName>
-    <definedName name="_xlchart.v1.65" hidden="1">data!$A$2:$A$63</definedName>
-    <definedName name="_xlchart.v1.66" hidden="1">data!$B$1</definedName>
-    <definedName name="_xlchart.v1.67" hidden="1">data!$B$2:$B$63</definedName>
-    <definedName name="_xlchart.v1.68" hidden="1">data!$C$1</definedName>
-    <definedName name="_xlchart.v1.69" hidden="1">data!$C$2:$C$63</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">data!$E$2:$E$63</definedName>
-    <definedName name="_xlchart.v1.70" hidden="1">data!$D$1</definedName>
-    <definedName name="_xlchart.v1.71" hidden="1">data!$D$2:$D$63</definedName>
-    <definedName name="_xlchart.v1.72" hidden="1">data!$E$1</definedName>
-    <definedName name="_xlchart.v1.73" hidden="1">data!$E$2:$E$63</definedName>
-    <definedName name="_xlchart.v1.74" hidden="1">data!$F$1</definedName>
-    <definedName name="_xlchart.v1.75" hidden="1">data!$F$2:$F$63</definedName>
-    <definedName name="_xlchart.v1.76" hidden="1">data!$G$1</definedName>
-    <definedName name="_xlchart.v1.77" hidden="1">data!$G$2:$G$63</definedName>
-    <definedName name="_xlchart.v1.78" hidden="1">data!$H$1</definedName>
-    <definedName name="_xlchart.v1.79" hidden="1">data!$H$2:$H$63</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">data!$F$1</definedName>
-    <definedName name="_xlchart.v1.80" hidden="1">data!$I$1</definedName>
-    <definedName name="_xlchart.v1.81" hidden="1">data!$I$2:$I$63</definedName>
-    <definedName name="_xlchart.v1.82" hidden="1">data!$J$1</definedName>
-    <definedName name="_xlchart.v1.83" hidden="1">data!$J$2:$J$63</definedName>
-    <definedName name="_xlchart.v1.84" hidden="1">data!$K$1</definedName>
-    <definedName name="_xlchart.v1.85" hidden="1">data!$K$2:$K$63</definedName>
-    <definedName name="_xlchart.v1.86" hidden="1">data!$A$2:$A$63</definedName>
-    <definedName name="_xlchart.v1.87" hidden="1">data!$B$2:$B$63</definedName>
-    <definedName name="_xlchart.v1.88" hidden="1">data!$C$1</definedName>
-    <definedName name="_xlchart.v1.89" hidden="1">data!$C$2:$C$63</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">data!$F$2:$F$63</definedName>
-    <definedName name="_xlchart.v1.90" hidden="1">data!$D$1</definedName>
-    <definedName name="_xlchart.v1.91" hidden="1">data!$D$2:$D$63</definedName>
-    <definedName name="_xlchart.v1.92" hidden="1">data!$E$1</definedName>
-    <definedName name="_xlchart.v1.93" hidden="1">data!$E$2:$E$63</definedName>
-    <definedName name="_xlchart.v1.94" hidden="1">data!$F$1</definedName>
-    <definedName name="_xlchart.v1.95" hidden="1">data!$F$2:$F$63</definedName>
-    <definedName name="_xlchart.v1.96" hidden="1">data!$G$1</definedName>
-    <definedName name="_xlchart.v1.97" hidden="1">data!$G$2:$G$63</definedName>
-    <definedName name="_xlchart.v1.98" hidden="1">data!$H$1</definedName>
-    <definedName name="_xlchart.v1.99" hidden="1">data!$H$2:$H$63</definedName>
-    <definedName name="_xlchart.v5.61" hidden="1">data!$A$1</definedName>
-    <definedName name="_xlchart.v5.62" hidden="1">data!$A$2:$A$63</definedName>
-    <definedName name="_xlchart.v5.63" hidden="1">data!$B$1</definedName>
-    <definedName name="_xlchart.v5.64" hidden="1">data!$B$2:$B$63</definedName>
-  </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="79">
   <si>
     <t>country_code</t>
   </si>
@@ -420,6 +264,21 @@
   <si>
     <t>ZWE</t>
   </si>
+  <si>
+    <t>satisfied_mean</t>
+  </si>
+  <si>
+    <t>p-value for Y</t>
+  </si>
+  <si>
+    <t>r2ZG − maxYˆ {r2Yˆ }</t>
+  </si>
+  <si>
+    <t>r2 ZG - r2 Y</t>
+  </si>
+  <si>
+    <t>r2 ZG</t>
+  </si>
 </sst>
 </file>
 
@@ -624,7 +483,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DFFE1104-E50D-9B4C-8586-5F354C48A44F}" type="CELLRANGE">
+                    <a:fld id="{9B325541-20C3-3E4C-93C3-130EFB175FA9}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -657,7 +516,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FCEAE319-96C4-5C4F-811E-2F4D6DA7F437}" type="CELLRANGE">
+                    <a:fld id="{65B31F05-4887-BB49-BD96-D263483372EA}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -690,7 +549,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{56043BC6-712B-0F4B-9D2B-AA8658CFA46F}" type="CELLRANGE">
+                    <a:fld id="{737B7752-7D93-C643-9D55-B4C3283BDA2E}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -723,7 +582,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2E1D33C0-9B37-074F-A3F0-68D64ADDBD26}" type="CELLRANGE">
+                    <a:fld id="{CE6F7204-FDBD-8646-B4D8-C8A9CD755DF1}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -756,7 +615,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A98E60C0-8346-2F41-AE4C-FF1A05F64763}" type="CELLRANGE">
+                    <a:fld id="{E6C3E0FF-AA1E-2B4C-A5EF-D603D6A636B7}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -789,7 +648,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B7A3E148-C56D-A84F-8B4E-3D361113D4CF}" type="CELLRANGE">
+                    <a:fld id="{12AF5736-BE69-0C43-B332-C84065C75557}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -822,7 +681,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1B80F133-6C0D-E64F-9C03-1F8B16B48892}" type="CELLRANGE">
+                    <a:fld id="{5E11B899-E56D-314C-AE3F-A4AE624CF302}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -855,7 +714,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0A1DAF07-675D-E34E-B5F6-7C80875E6E75}" type="CELLRANGE">
+                    <a:fld id="{3DE46D19-3B13-B447-8A60-9D58666CD1D0}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -888,7 +747,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2CFCFEA3-A09C-D048-AB5B-93C8961B415D}" type="CELLRANGE">
+                    <a:fld id="{964D20BE-857F-374F-B238-714DAC75FD76}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -921,7 +780,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{016601BE-E660-4743-9DB1-3A8257EB9AE8}" type="CELLRANGE">
+                    <a:fld id="{3D6AC566-F4DD-6F45-B798-83F1EAB3A272}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -954,7 +813,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9C96D6D3-814A-5640-A4CF-C32FE4ECB109}" type="CELLRANGE">
+                    <a:fld id="{A198D5EF-8FC2-9444-9EE6-192BDF788F61}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -987,7 +846,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CBBC5F1A-63A1-2C4A-81C9-39C4C9532F08}" type="CELLRANGE">
+                    <a:fld id="{65265FD1-6C72-1649-A6C4-6F76753B4B0B}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1020,7 +879,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AD4E7B35-0067-0E4D-B909-4E83354E70D9}" type="CELLRANGE">
+                    <a:fld id="{98202207-A57E-8242-9621-032E122F003B}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1053,7 +912,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D4302860-7299-9341-BED3-5E6AE275DB39}" type="CELLRANGE">
+                    <a:fld id="{36BC4699-72EE-1248-AC98-84D6216AF46C}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1086,7 +945,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1C83F7E3-5143-0146-8EF7-0ABEB33FB2C8}" type="CELLRANGE">
+                    <a:fld id="{962CDDAF-93D4-EE4D-A4C5-B0077F60A91D}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1119,7 +978,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2F74BD02-B13D-C84A-82B7-522A426D4367}" type="CELLRANGE">
+                    <a:fld id="{BC55F691-D3B6-6A45-8D59-0CFDD6E3DD1A}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1152,7 +1011,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1C9C73C6-B94C-0849-9219-86E3AF47DBCD}" type="CELLRANGE">
+                    <a:fld id="{59923BA8-F201-7B47-83BC-BFD2CC923882}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1185,7 +1044,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{24D51E2B-8687-5645-B547-2592BF09438B}" type="CELLRANGE">
+                    <a:fld id="{669E8DB6-B696-C64B-82C3-95587B358284}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1218,7 +1077,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7845917D-D0B0-FC49-8F5F-DF3747332F01}" type="CELLRANGE">
+                    <a:fld id="{E9F53FDF-76CE-7648-8DF3-F827FE71157B}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1251,7 +1110,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0AA95108-1102-B444-95E5-721F98921511}" type="CELLRANGE">
+                    <a:fld id="{861C01D3-0306-0842-90C9-8E6915A021EA}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1284,7 +1143,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B99BB27D-42AD-464C-8A71-D7D3E592ABED}" type="CELLRANGE">
+                    <a:fld id="{BE54DA6B-A6D1-AC4F-AC42-9232D7FE2160}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1317,7 +1176,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{ECF6FC97-4415-E34F-B75D-42C93084BCC5}" type="CELLRANGE">
+                    <a:fld id="{09BB5AE7-19D0-BB4F-854E-9FF9A7C51038}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1350,7 +1209,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1D7C12FD-9E61-844D-9FCC-B6A56692690F}" type="CELLRANGE">
+                    <a:fld id="{3EBF15E0-1EE7-FA44-8E5B-ED94501EEFDC}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1383,7 +1242,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8EBECB1A-01BE-154F-8FA5-50D19A1B19C0}" type="CELLRANGE">
+                    <a:fld id="{F3FFD28E-13E0-4A49-873F-D19FA9D7D1E8}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1416,7 +1275,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D2F23127-8A0D-FF47-A6E7-E96602B61192}" type="CELLRANGE">
+                    <a:fld id="{306FB6FA-34A9-8247-98FF-498F3DECE318}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1449,7 +1308,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DC5DAD7C-2497-7547-9071-A127BB8E1DD9}" type="CELLRANGE">
+                    <a:fld id="{B08FA5D3-5372-874E-8738-2EDB18FB63FF}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1482,7 +1341,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3BC365F7-D0AE-884B-902D-D97ED70AE515}" type="CELLRANGE">
+                    <a:fld id="{9AE7584A-1384-BA47-806F-2A348F1E377D}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1515,7 +1374,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A1A041ED-0B70-EA47-A188-B74175E1800D}" type="CELLRANGE">
+                    <a:fld id="{7A35DFB0-2080-A743-8F0D-5E1A55D7F925}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1548,7 +1407,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3D3A03DB-6A3A-6449-B29C-83F8B17FDCF1}" type="CELLRANGE">
+                    <a:fld id="{C6CD0F50-862C-214B-9C81-7DF6C7909886}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1581,7 +1440,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9581C933-3BB5-2142-B0E3-B611BA10B594}" type="CELLRANGE">
+                    <a:fld id="{8A547D95-589E-574A-ACB9-87FC3F5FE441}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1614,7 +1473,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7D81D698-E875-C144-8B54-B12F0E7DA3E5}" type="CELLRANGE">
+                    <a:fld id="{4EFDD1EC-D8FB-444C-8F9F-78E1D9E6FF3C}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1647,7 +1506,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{69559C54-03D0-F84F-8F48-EB6B2D1BFC4D}" type="CELLRANGE">
+                    <a:fld id="{29350A16-4885-A84C-B022-05DBB4BE1C17}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1680,7 +1539,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A546435F-5C3E-C043-8221-F4F2D474CC1E}" type="CELLRANGE">
+                    <a:fld id="{5B6C8067-03A1-2748-82AD-74C1B588EECD}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1713,7 +1572,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{83ACDFD2-2671-0F4A-A52A-7813246C68CA}" type="CELLRANGE">
+                    <a:fld id="{92FEDD94-8DEA-BB43-AEE2-F03FC6182928}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1746,7 +1605,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4E83E4C1-66D5-6F40-9C52-781423DC957C}" type="CELLRANGE">
+                    <a:fld id="{C6F58FEE-60F5-374D-A8D6-79C2A9A253C0}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1779,7 +1638,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DDC3E166-7457-4742-BE82-615EEB370229}" type="CELLRANGE">
+                    <a:fld id="{55E93F3E-0816-AF48-985F-0F83056A6236}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1812,7 +1671,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4BF5EAEC-16EC-1744-B067-4F1127158A49}" type="CELLRANGE">
+                    <a:fld id="{5D30529E-86FA-FA4B-8AB0-8DBB1FE11EAE}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1845,7 +1704,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E0B48819-3FF4-A341-B2CF-93FD850C55CD}" type="CELLRANGE">
+                    <a:fld id="{1AA3CEDF-1C5A-5249-924F-516C19914B16}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1878,7 +1737,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{070958D4-3230-6E42-9E84-9ACFA20D0E40}" type="CELLRANGE">
+                    <a:fld id="{0F73AAA9-CC22-2343-85C7-021D926BFFEF}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1911,7 +1770,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{716FA989-6CC7-EA49-AD5C-D0CE90F9B5F8}" type="CELLRANGE">
+                    <a:fld id="{A482D9AC-F287-B94E-A408-915F566465C0}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1944,7 +1803,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A7CE3D68-2AB8-6246-830C-F3B511075AB1}" type="CELLRANGE">
+                    <a:fld id="{E4E4BF46-BBA0-1941-8473-9A3F830D1139}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1977,7 +1836,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F4AF8C8C-2246-6C4A-BBC7-FDB82861AA7A}" type="CELLRANGE">
+                    <a:fld id="{0950128F-5785-DE42-8385-F690D4E204C2}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2010,7 +1869,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9BD9B0D0-81B2-294C-B1D0-259D8EA1CC30}" type="CELLRANGE">
+                    <a:fld id="{5435B8C8-6F6B-4240-B46D-75BD01E3E1D4}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2043,7 +1902,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EA0A8FFB-3CEA-E640-9722-22B5290EA344}" type="CELLRANGE">
+                    <a:fld id="{0FB60C29-A758-C048-8D70-CA7D0A04ED50}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2076,7 +1935,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6DE0D034-A555-D242-BF34-E7902DCB71F2}" type="CELLRANGE">
+                    <a:fld id="{D569F770-F178-0141-8713-9E0B222CFBD8}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2109,7 +1968,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FA34D83B-30DB-A44A-97DA-3CE0BCD50DEF}" type="CELLRANGE">
+                    <a:fld id="{29991B5D-CBAC-F848-B1AB-CD2920620F40}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2142,7 +2001,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C04BCB65-CD3B-6242-827C-9B7E865CAAEB}" type="CELLRANGE">
+                    <a:fld id="{0C7F75AA-FA0E-964B-AEC1-16D94E2C860C}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2175,7 +2034,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{789AE202-F653-B149-A5C4-6F272885354C}" type="CELLRANGE">
+                    <a:fld id="{7B8BE49B-C4C2-124F-88A4-19CD43E99BA6}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2208,7 +2067,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0557D263-87D6-3B41-AEFC-618BA4581149}" type="CELLRANGE">
+                    <a:fld id="{ACA61C38-DC86-BA4F-99FA-E1B638605C1A}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2241,7 +2100,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{067597E9-D17F-1441-83F3-8305DCFD92E7}" type="CELLRANGE">
+                    <a:fld id="{5F1A4C46-8E11-2C40-A4F5-66621C73677E}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2274,7 +2133,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0D62DE61-401D-3D43-824A-B9143A5DB845}" type="CELLRANGE">
+                    <a:fld id="{85AE620C-DF1B-184F-BFCB-64855144C99D}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2307,7 +2166,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BC12A608-C40B-EA4E-A6EF-1FF3FC3E578C}" type="CELLRANGE">
+                    <a:fld id="{F1BD7A89-66F1-C74F-A8DE-3C6CBEA7DAE6}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2340,7 +2199,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8262856D-5EDC-9947-A88F-7AFDFF6A68B0}" type="CELLRANGE">
+                    <a:fld id="{960CBC12-182C-ED42-BB8B-088CF4C9D0B5}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2373,7 +2232,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{042C1463-7A99-684E-BE3E-7778FD042833}" type="CELLRANGE">
+                    <a:fld id="{0BECC0C7-0531-BB47-AA63-7C674E7047CF}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2406,7 +2265,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6CF0BABB-BF83-1B41-86C2-B228F9D6A82F}" type="CELLRANGE">
+                    <a:fld id="{EE70F31B-1FBD-1042-A7D4-F6E9B1E620F5}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2439,7 +2298,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F2E07CA3-F5AE-8D40-A327-6E4BAE25C87C}" type="CELLRANGE">
+                    <a:fld id="{2D27305A-6F53-3F4D-B7BD-8B5F8AD8A4EE}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2472,7 +2331,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1222E6B4-8AA7-DD41-B695-4DD7B1BCE912}" type="CELLRANGE">
+                    <a:fld id="{EF54A135-43CB-1E4F-80EC-AC5DB390B055}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2505,7 +2364,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{34C60BFC-CB62-5244-BB9E-8F9E8FB040C8}" type="CELLRANGE">
+                    <a:fld id="{8F0F5416-3F48-5E42-8AD3-5E9444291916}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2538,7 +2397,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6604F958-22AA-8C45-94FC-BC4F06B97D7F}" type="CELLRANGE">
+                    <a:fld id="{9038CDD9-C9A1-9744-A19B-BB2D05A65E39}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2571,7 +2430,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A9469D13-668D-2C4A-A71F-1D14A3E54D0A}" type="CELLRANGE">
+                    <a:fld id="{8FB4E055-507E-9745-AE06-0BB7E46A9FCF}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2604,7 +2463,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D37E8F51-C908-2F46-BD8A-14ED6674E0DD}" type="CELLRANGE">
+                    <a:fld id="{F516E621-AE36-3241-924A-14D0D7B8704D}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3706,7 +3565,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2F164D76-E9C4-314B-9F8E-0F22BFE0D595}" type="CELLRANGE">
+                    <a:fld id="{FB0052B1-783B-DF41-B0C7-9B6CAB94276D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3738,7 +3597,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{79FC05F8-F125-8C43-BBDD-5D5B78219AC1}" type="CELLRANGE">
+                    <a:fld id="{30B7C8C8-6FF7-3C40-94E8-D0479F5AC34D}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3771,7 +3630,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5396A4A8-78F0-404E-9580-D156F305E21E}" type="CELLRANGE">
+                    <a:fld id="{509F2A9D-7023-FE4A-BBBC-A9947BE0C7AF}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3804,7 +3663,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CFA31F39-9FD1-B54B-84C2-42D03CE890C0}" type="CELLRANGE">
+                    <a:fld id="{2F02A12E-2B33-B24A-A66F-5F8823B79D74}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3837,7 +3696,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1742B996-0674-2349-9F98-D7688D43B3D7}" type="CELLRANGE">
+                    <a:fld id="{983A99E1-49B5-1B42-9ADB-DB6FB491EC6E}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3870,7 +3729,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F75320A7-699E-5D4F-841B-467C3A2BAEFA}" type="CELLRANGE">
+                    <a:fld id="{7EDE73E9-B402-8B43-9A83-47E2C8534D6F}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3903,7 +3762,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{21D453B0-A9E0-1646-9703-1B8E0BFC4D5A}" type="CELLRANGE">
+                    <a:fld id="{54CBFEB4-40EA-524C-93A6-333C70FCDC47}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3936,7 +3795,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E13ECC4B-BED8-EC44-A8C3-5E02B1900977}" type="CELLRANGE">
+                    <a:fld id="{DE864574-0A42-4941-9E1C-8B2C6D104D1A}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3969,7 +3828,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{45A65F01-B7F9-1844-B762-9DE592F1FF82}" type="CELLRANGE">
+                    <a:fld id="{36B827CA-7A91-794F-9FFF-784E21118AEA}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4002,7 +3861,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4AC539D2-1F32-C248-A733-4B4D9185360F}" type="CELLRANGE">
+                    <a:fld id="{908B7CAB-F72C-A342-B381-09A00F4107E4}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4035,7 +3894,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5A57FED7-8AC5-1240-86F8-2ABC5D84F447}" type="CELLRANGE">
+                    <a:fld id="{5608D11E-294F-AC44-847C-F3106A24688F}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4068,7 +3927,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DA425052-0EF8-7243-B23E-DE61FFE118FA}" type="CELLRANGE">
+                    <a:fld id="{9343989F-C9A6-224A-92DA-6AB64EBAF9D9}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4101,7 +3960,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CD3B7B5E-AFEC-AD4A-AE52-971E66F100E5}" type="CELLRANGE">
+                    <a:fld id="{36FB7133-0159-994B-ACF3-646D51509801}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4134,7 +3993,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{57CCB1B6-DAEE-AC4D-8B70-52A28A6C1D3E}" type="CELLRANGE">
+                    <a:fld id="{CF7181D3-9BFB-8049-B652-615BFB52328C}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4167,7 +4026,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{22F16013-4792-8B4A-9714-DC0BA74BB7C1}" type="CELLRANGE">
+                    <a:fld id="{866BC2E5-601C-0242-8C57-19607FCB0274}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4200,7 +4059,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C7003378-FA0C-0742-A316-54D1515D14CE}" type="CELLRANGE">
+                    <a:fld id="{898E5B95-1F6A-BE43-90FD-4180BD96977D}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4233,7 +4092,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{29AB0A60-9BED-C147-B61F-68061CD0E410}" type="CELLRANGE">
+                    <a:fld id="{1492CFE5-E7DD-F140-9BCD-15F2F9FA7271}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4266,7 +4125,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2CD5A29C-9921-9640-B986-5B6305FE6848}" type="CELLRANGE">
+                    <a:fld id="{E892D3AE-CF22-534D-8FB0-614B21FCE36F}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4299,7 +4158,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E7B83061-564C-C540-8D5A-A1897C1BE3F3}" type="CELLRANGE">
+                    <a:fld id="{DF4F74E8-45B3-6B4A-8D08-243CE881A706}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4332,7 +4191,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{890603B2-02A5-FC43-99F5-E92A5475D4E2}" type="CELLRANGE">
+                    <a:fld id="{28EE1C59-4E2F-7344-9E72-2AABC959831C}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4365,7 +4224,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{921B6EA4-5F90-B349-98A4-F6E489380D54}" type="CELLRANGE">
+                    <a:fld id="{02AC0861-C1EF-4144-8628-B6556A54CEEB}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4398,7 +4257,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E09FC318-F8A3-FF44-8F1A-4FF637BB64D1}" type="CELLRANGE">
+                    <a:fld id="{10D6502B-52BA-074D-A5EA-5479F35CDEDC}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4431,7 +4290,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B94D4164-1179-E449-AA1B-267B2C8957B0}" type="CELLRANGE">
+                    <a:fld id="{2BC764D2-4FEC-F945-8658-72E070C8D217}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4464,7 +4323,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5606F808-A165-2B49-8875-CFB8D3404B01}" type="CELLRANGE">
+                    <a:fld id="{93A51FF1-C5BC-F340-8F4B-87E3F3EC8F07}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4497,7 +4356,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7C24BCCF-39E7-E843-975A-9CDB78B62A98}" type="CELLRANGE">
+                    <a:fld id="{C18DA70F-4E99-6143-A3A8-CEBF0277A7A2}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4530,7 +4389,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B284479A-3863-B14C-B01B-21CCCAEBA901}" type="CELLRANGE">
+                    <a:fld id="{1EB4D482-019E-6B47-A2BA-87709973C123}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4563,7 +4422,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3F98A1CE-C535-1242-AB34-3B0E7E3C19FC}" type="CELLRANGE">
+                    <a:fld id="{39CF7D0F-DC69-2D44-B4A1-D86E607C7DA5}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4596,7 +4455,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AF38FD99-D74B-3146-BEC9-4552A0C99A5A}" type="CELLRANGE">
+                    <a:fld id="{8D382B8E-F356-014B-8979-6430AAEDAB37}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4629,7 +4488,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CD2F90B8-8D71-E447-AB47-166E7E018E65}" type="CELLRANGE">
+                    <a:fld id="{895BB6AE-7DFE-BC42-8370-7BEBB26E3873}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4662,7 +4521,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5F1840E4-6A0B-FD4F-A47E-AB1D2987D2B9}" type="CELLRANGE">
+                    <a:fld id="{FA576FAF-8E3A-2141-88C2-7EC76F630475}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4695,7 +4554,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7F757044-AD19-3B43-96C0-0488DF529763}" type="CELLRANGE">
+                    <a:fld id="{075B6EF0-B6B5-F54A-BF6B-9EFF5E1CDAD6}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4728,7 +4587,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BEE86AE5-D602-C344-8504-F0A168CE16FB}" type="CELLRANGE">
+                    <a:fld id="{D202B483-4E1B-0A4E-A7A9-35B0927D9352}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4761,7 +4620,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CE8CD8B5-D509-9447-9BB0-2D7E33CDF100}" type="CELLRANGE">
+                    <a:fld id="{70D8454F-3EF4-724D-8512-3805FCDA26C6}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4794,7 +4653,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5B8D17D6-5748-C242-B6D9-633E4F227819}" type="CELLRANGE">
+                    <a:fld id="{8D9FC2D6-CCCC-DA47-B9BA-DCBA99F2FFE1}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4827,7 +4686,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1EE93B19-86B7-8A4E-8D4D-FBA491ED94AF}" type="CELLRANGE">
+                    <a:fld id="{A17E30D8-2AF1-1148-8530-5FABF0D3438B}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4860,7 +4719,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{79850094-A0A5-864B-80ED-84DF26C347BF}" type="CELLRANGE">
+                    <a:fld id="{0A00B976-69F4-0E41-8D77-21AC9274AD92}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4893,7 +4752,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7FF90232-4F10-6B43-9C3A-40AACAA62260}" type="CELLRANGE">
+                    <a:fld id="{F12794F6-1AD9-F042-BFDF-5E814B4C1D2F}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4926,7 +4785,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4AE845E2-019A-F448-8947-8765F61C86D1}" type="CELLRANGE">
+                    <a:fld id="{D91EF14F-6EF9-984B-9C20-31D15671F06D}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4959,7 +4818,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2397057C-9D21-8A4A-9876-61039F5FD01F}" type="CELLRANGE">
+                    <a:fld id="{FE1BC37B-A314-E845-88B7-711460D13CB9}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4992,7 +4851,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{163ED8B8-FC56-FA48-9CDD-4D9800013BB5}" type="CELLRANGE">
+                    <a:fld id="{84723AEE-E579-5D48-8CFB-455D2E496D0B}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5025,7 +4884,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6E7DFC68-6839-0045-97F4-316D83A756C0}" type="CELLRANGE">
+                    <a:fld id="{5F1C691B-B347-DB45-B486-651643E92D77}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5058,7 +4917,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{20E4746C-8B7D-5D4A-8A5D-C107D87DE257}" type="CELLRANGE">
+                    <a:fld id="{63AF023E-ECD9-7F44-8F16-211F4ED5B102}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5091,7 +4950,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{80B99FC9-9C2A-0A4C-BC3E-5CB7F7F8CBD5}" type="CELLRANGE">
+                    <a:fld id="{5C5003C0-2677-A546-9C99-89DD8CAE63DF}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5124,7 +4983,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D0434033-C687-DB45-AD41-218B9EAC7902}" type="CELLRANGE">
+                    <a:fld id="{40ED4355-F0FF-7747-9D11-A35293B4C0E8}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5157,7 +5016,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8EEA32D1-FE85-A94A-A2C9-DA630A707A86}" type="CELLRANGE">
+                    <a:fld id="{2BC498E3-D5AA-6A44-AA66-E4BD23395ED7}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5190,7 +5049,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A4C72E3C-2DEC-9744-889B-A83E8F45B1A7}" type="CELLRANGE">
+                    <a:fld id="{4455D0DE-83EF-D848-84F1-272180987AC7}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5223,7 +5082,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{99950539-D4B9-1D4F-834F-61A833EF8236}" type="CELLRANGE">
+                    <a:fld id="{929EA3B2-391B-9145-A68F-8E1043FF68C7}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5256,7 +5115,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CCDAA2DA-6469-D048-869B-7657BF1C9B82}" type="CELLRANGE">
+                    <a:fld id="{11C63338-9B97-F640-AAA0-D61C5BFC9819}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5289,7 +5148,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A08F7F6B-4E03-E442-82B2-E3F14D007995}" type="CELLRANGE">
+                    <a:fld id="{5958BE27-6887-FB4B-A6BC-03C5E42205F6}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5322,7 +5181,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{88137C69-5A0B-E749-83CE-3E160DE118F3}" type="CELLRANGE">
+                    <a:fld id="{F1EAFCC6-1159-8F46-9287-BB4DE39BDFDA}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5355,7 +5214,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B0B8400C-6608-FE41-8136-0657F35AAF66}" type="CELLRANGE">
+                    <a:fld id="{87C9FA21-9AEE-F448-8C0A-7D062C63D7EB}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5388,7 +5247,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4626AEA4-198E-EA45-A8F6-9DF507688CAD}" type="CELLRANGE">
+                    <a:fld id="{C4B741CF-C829-F640-B431-F7AD9FC7A4D8}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5421,7 +5280,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F33345DD-0F4A-E547-9204-6B893AE6B22A}" type="CELLRANGE">
+                    <a:fld id="{5B15CC7B-E523-4F49-B9EC-91F03C94FEB0}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5454,7 +5313,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B2B486BB-327E-2E47-A13B-25BB82092894}" type="CELLRANGE">
+                    <a:fld id="{2666F002-AFEF-6E43-8446-7E8A547E1BFE}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5487,7 +5346,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B0072652-653F-4649-B245-4E80695F8108}" type="CELLRANGE">
+                    <a:fld id="{27C0A026-37AD-4C48-91A4-9E1362FC0BEF}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5520,7 +5379,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CED3DD68-10EC-D74C-8702-BBA8A3CC114B}" type="CELLRANGE">
+                    <a:fld id="{E0F5A021-73C9-E241-9017-E33A2D0E69E7}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5553,7 +5412,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0C8A14EA-B2D2-0F46-849F-7E1BBC3E8CB7}" type="CELLRANGE">
+                    <a:fld id="{EC796708-5A78-6649-8D0C-FA61304048D2}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5586,7 +5445,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{550CDBDE-9CD1-EB4F-8625-548D408CE791}" type="CELLRANGE">
+                    <a:fld id="{9637A70C-C75E-5046-8510-15FC5D3341C8}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5619,7 +5478,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{56F61FAA-B573-664E-B6F5-CCFAEF8E0B9F}" type="CELLRANGE">
+                    <a:fld id="{C83B40B4-EAC0-FF45-9D28-8042640F0C69}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5652,7 +5511,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AA2D9523-FCCA-7848-9F2E-A3720C8FFB75}" type="CELLRANGE">
+                    <a:fld id="{611FA899-4CBA-3B4B-8C9F-AA462F94770F}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5685,7 +5544,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DCDBD1C8-E338-9F41-A373-484FE02F7B4A}" type="CELLRANGE">
+                    <a:fld id="{E6A8E0D2-5AB3-CA4C-B3E0-24586E3D71F0}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5718,7 +5577,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{95A18F48-E611-FA46-88AA-98D6EE867689}" type="CELLRANGE">
+                    <a:fld id="{61080B81-8FFC-DE40-9093-497F01591374}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6871,7 +6730,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B549F53D-C7E8-8B45-BD6E-474612A6B221}" type="CELLRANGE">
+                    <a:fld id="{57A53282-26F4-BB44-8E88-B4C1CA9389EE}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6904,7 +6763,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{075B529C-3B19-3B47-A715-7C5294889D21}" type="CELLRANGE">
+                    <a:fld id="{8F4AA789-CCA9-7B4A-B7C6-0FB26EAA02EB}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6937,7 +6796,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0EDFBF13-0CBA-414B-8ED2-99BFB4DDF832}" type="CELLRANGE">
+                    <a:fld id="{91E2F5E7-4919-8D42-B6C5-F47652D51FB0}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6970,7 +6829,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{64D98EF3-6CD6-9E4B-B7E7-D079FFF85CF9}" type="CELLRANGE">
+                    <a:fld id="{75D92B9D-50FD-CB44-A4B8-EDDEFDE28D5F}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7003,7 +6862,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E8B26BE2-5A19-CA49-8041-11375593EF03}" type="CELLRANGE">
+                    <a:fld id="{40D73415-5E30-E146-85B0-B07E70C1AB97}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7036,7 +6895,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{467CAEA0-1FE3-C641-BF41-AF6CED227D16}" type="CELLRANGE">
+                    <a:fld id="{68F72EE5-187C-5F4B-9019-461FF1C13CB3}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7069,7 +6928,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D3D1DE6D-6480-BE41-96BD-348FCDC938B3}" type="CELLRANGE">
+                    <a:fld id="{C59BCAC9-7566-9041-92C2-92D79D06C815}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7102,7 +6961,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6F5D7E7C-8A84-FC49-9FD2-9E1AB039E1DF}" type="CELLRANGE">
+                    <a:fld id="{1952C42F-E492-3140-8F71-33712394C764}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7135,7 +6994,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AD61D3D2-2996-FF49-BCB7-625ADD98B83E}" type="CELLRANGE">
+                    <a:fld id="{6CB00B4F-06B9-2D4D-B0DC-51CF2EF5A8A8}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7168,7 +7027,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D672FD4C-43DF-434E-B13F-5342A5A5B7E4}" type="CELLRANGE">
+                    <a:fld id="{03284A1F-B4B1-FA4E-8CFD-E5655CC35E6F}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7201,7 +7060,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3CCFD95D-DF2F-DB4D-AA65-0C9A6618FCBE}" type="CELLRANGE">
+                    <a:fld id="{CEEC8A2B-7BD3-B04B-85C9-457CF395F25C}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7234,7 +7093,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2309916C-85E7-0C43-96C1-4FE00C278B6B}" type="CELLRANGE">
+                    <a:fld id="{71EBFE60-2F7A-0B49-8127-F332ADF98892}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7267,7 +7126,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B815D946-FBCF-6D44-918E-ADCF97A42812}" type="CELLRANGE">
+                    <a:fld id="{21AE3C7C-2B47-D945-8DDC-1408D2101458}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7300,7 +7159,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C0EDF097-E9BB-DE44-84A8-859FFCB7F8FC}" type="CELLRANGE">
+                    <a:fld id="{66F7924C-0002-5949-BDEF-AA15D6CE670D}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7333,7 +7192,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CEE18234-6484-9F43-B43A-F7FF310BD030}" type="CELLRANGE">
+                    <a:fld id="{7FE6F026-9A5F-1942-B535-E560AB4D27DD}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7366,7 +7225,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EAA152D4-E989-C244-8EC1-8E7A1F3358A8}" type="CELLRANGE">
+                    <a:fld id="{AFE20A5B-51F3-2147-9624-2C57EDF5BF3C}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7399,7 +7258,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{920E9F01-AA7A-6F44-87C7-0A861D862735}" type="CELLRANGE">
+                    <a:fld id="{E25B1E4B-9021-7345-80F3-2607CB247CDA}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7432,7 +7291,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B7F9C335-6068-EB40-8558-715BFADE4CF5}" type="CELLRANGE">
+                    <a:fld id="{213FE6F9-3BDA-5C44-B48E-21C39788469F}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7465,7 +7324,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{71321FA2-11C7-F943-A107-05BD02B06AB0}" type="CELLRANGE">
+                    <a:fld id="{058DD432-8096-DB48-A993-967D8FD70AB7}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7498,7 +7357,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1640CA21-04A2-1145-A2E2-4BE4BCFCB41F}" type="CELLRANGE">
+                    <a:fld id="{CF12CD42-94AE-1043-8BAA-8DBF8E238D58}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7531,7 +7390,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BA55FE6E-40AE-1742-A079-6D2CC290C4B0}" type="CELLRANGE">
+                    <a:fld id="{42DD0598-2570-3F4B-AE5B-AD090AC263BB}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7564,7 +7423,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2E51B5D5-0792-BF43-AF10-2D95A5807C86}" type="CELLRANGE">
+                    <a:fld id="{5608EC4F-D5ED-184F-A3FB-28C0E15EC87E}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7597,7 +7456,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{65768AD0-1F71-1F47-8CBD-F7446014A4AD}" type="CELLRANGE">
+                    <a:fld id="{0BDACE34-DBF0-0944-A7FD-58368B29325E}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7630,7 +7489,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{24179943-9AD6-194A-9B1E-62FCA6D25DF6}" type="CELLRANGE">
+                    <a:fld id="{B0CECDD0-96AA-9648-A716-5CA2B1CD172C}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7663,7 +7522,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{02848240-FF95-904B-B113-F337D6E96B3B}" type="CELLRANGE">
+                    <a:fld id="{70568BBF-ED64-5549-AE76-D7486549253D}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7696,7 +7555,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{97AE60E7-ADA4-584F-BBAB-28EF524FA07E}" type="CELLRANGE">
+                    <a:fld id="{338AA302-1C8C-9041-93E6-D25A11696068}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7729,7 +7588,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A09CD905-F4F3-B749-B195-E5BAEA32C4BF}" type="CELLRANGE">
+                    <a:fld id="{F0EB6067-AE3B-6F46-B74B-E23DEAC0B629}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7762,7 +7621,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{40247087-D8B5-1243-AC31-93DCE9E42DCD}" type="CELLRANGE">
+                    <a:fld id="{0C35A16D-0E83-464A-AF4F-340457EF0103}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7795,7 +7654,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EA4BE60C-A561-B04F-8A0F-B2BAF0036BE2}" type="CELLRANGE">
+                    <a:fld id="{E3287A97-CF46-FA43-B783-02E3B93F2865}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7828,7 +7687,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0016D8BD-6211-F04B-89EC-68013788A981}" type="CELLRANGE">
+                    <a:fld id="{D1D2BED7-BD66-BE49-B030-9763795AF9D6}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7861,7 +7720,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A782A2C0-7469-204E-BBC3-F739727C8C96}" type="CELLRANGE">
+                    <a:fld id="{9240186D-19B0-C54E-A1D2-E0AD17585881}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7894,7 +7753,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{68C041C9-DCFC-E94F-86DC-A9735747925D}" type="CELLRANGE">
+                    <a:fld id="{9801BFB1-11BF-BF40-A453-153024CC6842}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7927,7 +7786,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{93BCD271-762F-8143-8E25-24605833ABF7}" type="CELLRANGE">
+                    <a:fld id="{C9F015C8-7CDA-744F-BED9-177EA2BD3E73}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7960,7 +7819,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5D31184A-38EF-B74E-BB4F-F74C40CB0788}" type="CELLRANGE">
+                    <a:fld id="{445E2015-C1E7-4A4E-989E-4A336752BFA6}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7993,7 +7852,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F95CAB1F-4FBC-6F4C-8E23-55C3EC6C4C4A}" type="CELLRANGE">
+                    <a:fld id="{741818BD-7205-244B-A0F8-AC5FC03C3FAF}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8026,7 +7885,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F9D19FA9-8EC6-9E4B-B3E9-BE652085F6E9}" type="CELLRANGE">
+                    <a:fld id="{92A37623-DB8E-7440-8FC4-FB78C90A8370}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8059,7 +7918,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4D65DDF0-0940-8B48-AC0A-E32AC5FE37AE}" type="CELLRANGE">
+                    <a:fld id="{EC53412B-55F3-F046-9C18-6CC14B216249}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8092,7 +7951,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7CD7533C-C51D-3E4B-9140-EDD365892107}" type="CELLRANGE">
+                    <a:fld id="{86575E32-01AE-2E4B-A839-5D281F58291E}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8125,7 +7984,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{503298B9-847D-F84B-90BE-4E41FB8538FF}" type="CELLRANGE">
+                    <a:fld id="{654FDA55-0115-EB49-8DFF-CD9335E5E97C}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8158,7 +8017,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C6DFFC78-5861-1041-A2B5-01278651A5DA}" type="CELLRANGE">
+                    <a:fld id="{F1327A27-7A69-5244-9B31-CC17CD44FDC4}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8191,7 +8050,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{54EE3CAB-67FB-6E42-9FB4-FDFBA10CFCC9}" type="CELLRANGE">
+                    <a:fld id="{4DE925A7-6304-704A-9673-10E6F7A947A3}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8224,7 +8083,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5A3E4762-CBF0-A949-AEB7-F0F319B1D87E}" type="CELLRANGE">
+                    <a:fld id="{16FFDABB-A35A-AA48-93A2-561ED9AC1AFD}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8257,7 +8116,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{11CC8E54-50AB-FD4A-8FBB-91F8763E24F2}" type="CELLRANGE">
+                    <a:fld id="{3A1F96DE-4FC7-EF42-B76B-C80A9638D1AF}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8290,7 +8149,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FCAF367F-01FB-EC42-A57C-6511F2FE28FD}" type="CELLRANGE">
+                    <a:fld id="{C2699B9C-4718-C34F-A6D0-802D27EB557E}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8323,7 +8182,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{40750195-74E7-1042-A5D2-98E8B193222F}" type="CELLRANGE">
+                    <a:fld id="{AF104FA6-685F-C94E-8D90-AE97759C5CD1}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8356,7 +8215,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DCEF6503-14C0-214B-B4CA-5CCD2C87D4B3}" type="CELLRANGE">
+                    <a:fld id="{FE8149BE-0F8A-384C-BEFF-EA64BC5B1B85}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8389,7 +8248,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9061C333-FBE9-5D4E-8FD8-0670D9339524}" type="CELLRANGE">
+                    <a:fld id="{AEAA15A8-05CB-4B4C-8A9B-3D087EFB498E}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8422,7 +8281,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E6C8A767-AB8D-EA43-B89F-AE198A4572AB}" type="CELLRANGE">
+                    <a:fld id="{23D206D9-AACC-3E42-A181-BD70F5FE5C6C}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8455,7 +8314,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{208982D1-5498-3A4B-AF2A-234DAFA294BC}" type="CELLRANGE">
+                    <a:fld id="{36C4369B-6D15-7A4C-A5ED-A22080E2DFC6}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8488,7 +8347,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6FC54BBA-F581-844D-AC10-3FFD0C7B2914}" type="CELLRANGE">
+                    <a:fld id="{417BD0AF-965C-7746-BB0B-FB347BF8EFDB}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8521,7 +8380,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D0368C73-4EE1-D24B-8E35-281EA36AB7F5}" type="CELLRANGE">
+                    <a:fld id="{619387B8-7162-544B-AE56-C37AB7382513}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8554,7 +8413,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C9D81BB6-BC42-424D-8684-4C1EC0A8CA6A}" type="CELLRANGE">
+                    <a:fld id="{5BC0C30F-12D2-F347-8457-E2F2CE2EA8D8}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8587,7 +8446,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A376DC47-B6E1-6846-876A-82F5E6098D2C}" type="CELLRANGE">
+                    <a:fld id="{4AE9143E-DE8E-0344-964D-384C6E7611F9}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8620,7 +8479,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7A19C635-4D48-FC42-8A13-87BBCB911DF9}" type="CELLRANGE">
+                    <a:fld id="{E481BD9F-8BE0-7648-B032-8AB09FBF6D78}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8653,7 +8512,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{718DF758-13EF-0445-BF81-022BAAF5C092}" type="CELLRANGE">
+                    <a:fld id="{82761871-229A-C040-B033-623EBCC9A14A}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8686,7 +8545,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EC4F4117-D532-2846-9F2D-E99B6A6B706C}" type="CELLRANGE">
+                    <a:fld id="{7B799273-B949-F246-B014-12281E966982}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8719,7 +8578,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{850D3745-9DAE-924E-AB19-2612B854653B}" type="CELLRANGE">
+                    <a:fld id="{36B39870-4C5B-BE40-B12D-C7B511AECB47}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8752,7 +8611,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{824DA0E6-361B-1146-8B08-E32EF788BBA6}" type="CELLRANGE">
+                    <a:fld id="{1303F406-7548-734F-BD6C-D685A65DAB64}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8785,7 +8644,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B399C433-1666-0347-9ED8-2B53BA60A4FB}" type="CELLRANGE">
+                    <a:fld id="{C4540988-FCC9-814C-B16F-DA9A4977A068}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8818,7 +8677,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A315EBE2-5AEA-A540-BA26-C7F556FE93F5}" type="CELLRANGE">
+                    <a:fld id="{888D9A74-7368-E342-A4B0-2126695B6A18}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8851,7 +8710,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3673147A-6F09-5E43-B18D-3470AC3019B7}" type="CELLRANGE">
+                    <a:fld id="{C6E9117B-4177-2D4A-AD22-1CC0E7FE340A}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9990,7 +9849,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DF3D083F-721C-5E49-B363-7037783CE200}" type="CELLRANGE">
+                    <a:fld id="{9108BEA6-FD22-9842-BFDC-A2CA05E65EA7}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10023,7 +9882,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BCED4BAE-718F-3C4E-AFF1-AC51E9435F49}" type="CELLRANGE">
+                    <a:fld id="{B1EB9811-013D-AF4D-8043-99C1206771E5}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10056,7 +9915,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2C087EB3-97A8-BB43-B7B4-9832B935C657}" type="CELLRANGE">
+                    <a:fld id="{FBEED8B9-952B-0140-AE31-69584092552B}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10089,7 +9948,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E668F60A-A51F-B741-AF0D-2EBADB4CDDCD}" type="CELLRANGE">
+                    <a:fld id="{C64BFB7C-2237-484B-AEC1-BBA49647B94C}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10122,7 +9981,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F1C87942-A5B4-BB4A-B13F-24C103CB58F3}" type="CELLRANGE">
+                    <a:fld id="{D9454237-74C9-3249-8B4C-B0C9FCA9DE47}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10155,7 +10014,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CB3AC8FB-D450-4F4B-979B-CF8596110878}" type="CELLRANGE">
+                    <a:fld id="{85AB67BC-7B20-394A-B4D4-DCDEC5580F85}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10188,7 +10047,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A20EEEEE-B999-784B-B702-EB8007A93B44}" type="CELLRANGE">
+                    <a:fld id="{D644D147-017C-1C4B-812D-99BF77A42E6B}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10221,7 +10080,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FAB0BFAB-0095-E343-B3AD-B19894C49ECC}" type="CELLRANGE">
+                    <a:fld id="{041E2F0B-2556-B745-92EC-58C6F02D3329}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10254,7 +10113,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A055840D-34D9-1E4D-8797-F0CB83589130}" type="CELLRANGE">
+                    <a:fld id="{DE7617B4-A3B4-704E-956D-B90E45B058DB}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10287,7 +10146,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{865CBE40-0C59-1342-A4DB-77CF835E79D0}" type="CELLRANGE">
+                    <a:fld id="{9C9A4802-C58A-EF4C-957D-DFE31745E871}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10320,7 +10179,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CB2E50DC-F2B2-A749-945F-9A9C007BF6BA}" type="CELLRANGE">
+                    <a:fld id="{7EC5DB60-3DD5-B445-A46C-0016B99E3557}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10353,7 +10212,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{779664C5-E93E-7E45-9535-7E46173862D9}" type="CELLRANGE">
+                    <a:fld id="{78EFE5AF-7AE1-F945-8249-DCA6DE0B65F8}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10386,7 +10245,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{06B856AE-CD62-764A-8E5E-91389AB2CE2F}" type="CELLRANGE">
+                    <a:fld id="{729899F0-78C4-EC41-B0BE-C73DAC167358}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10419,7 +10278,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{71B88F7B-B675-5143-AC2C-5C6CE639E868}" type="CELLRANGE">
+                    <a:fld id="{70C26C8F-FE51-5348-830C-CACAA00A2C57}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10452,7 +10311,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C219ED39-3529-1745-8FA2-66F763E576DE}" type="CELLRANGE">
+                    <a:fld id="{A77E419F-AEC4-784E-89A0-B4113E9A0CDD}" type="CELLRANGE">
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10461,7 +10320,7 @@
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:t>; </a:t>
                     </a:r>
-                    <a:fld id="{AE99AE08-7BB2-8A47-8CBF-F02983A009FA}" type="SERIESNAME">
+                    <a:fld id="{CA6248BE-58E9-1E45-A995-1C9B13EAF5CC}" type="SERIESNAME">
                       <a:rPr lang="en-US" baseline="0"/>
                       <a:pPr/>
                       <a:t>[NOMBRE DE LA SERIE]</a:t>
@@ -10493,7 +10352,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3F84C253-5836-AF47-8B34-2B19154DB16C}" type="CELLRANGE">
+                    <a:fld id="{1E6F62B2-E52C-904D-A922-94EEF9DCF816}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10526,7 +10385,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3E662F38-53D9-9D4C-BB77-70AF71481011}" type="CELLRANGE">
+                    <a:fld id="{538DCF11-E627-394F-AE03-666720F78BEF}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10559,7 +10418,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3F45D555-BE78-3344-9CED-00036D8AB086}" type="CELLRANGE">
+                    <a:fld id="{FDDB1AFB-B265-C849-8D18-339CCA301205}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10592,7 +10451,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{18F88D74-DE3E-4E47-A4CA-5F8086200EC3}" type="CELLRANGE">
+                    <a:fld id="{50CF2B5C-B8D4-F249-A43F-88A77B10EA43}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10625,7 +10484,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9821BC1C-F673-7549-888D-328388AAF2CB}" type="CELLRANGE">
+                    <a:fld id="{DCA624CA-BC8B-4641-B955-81C2C86DE109}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10658,7 +10517,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9BDEB4B5-9E1B-674B-B88A-634E9E3C22D9}" type="CELLRANGE">
+                    <a:fld id="{D0C926A4-004D-904B-92FC-7B8DAC32F1F4}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10691,7 +10550,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EAC521B3-C633-2A4F-B9CB-95264012E13A}" type="CELLRANGE">
+                    <a:fld id="{E1BF74BE-4E19-7F4B-9665-C19DDD148A76}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10724,7 +10583,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{038DAA39-8B57-CA4B-B907-71E000B7CDE1}" type="CELLRANGE">
+                    <a:fld id="{B788CB6B-2092-DE40-A50C-A9CBDB3B13CC}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10757,7 +10616,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E45BF865-41DC-A643-9DAE-E5DA6B397F86}" type="CELLRANGE">
+                    <a:fld id="{E1671BA7-F2D1-754A-8AC6-A7E8DEAEA703}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10790,7 +10649,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0995257F-5C36-864A-BC7E-CB189B3E49C2}" type="CELLRANGE">
+                    <a:fld id="{20D49CA5-340D-B045-8BED-15DC6F3DF59B}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10823,7 +10682,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0903BD7D-E2C4-EC41-B237-33983E145460}" type="CELLRANGE">
+                    <a:fld id="{052E1191-575C-CD4A-BB2B-6A2C10D9008E}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10856,7 +10715,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7BD22B69-F5A4-764A-A83D-EFC0D2F5A647}" type="CELLRANGE">
+                    <a:fld id="{0800EEC4-B3DD-564B-8A0A-BDC73AD59409}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10889,7 +10748,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{18F0D74C-7085-C74A-B772-9B4CF823555F}" type="CELLRANGE">
+                    <a:fld id="{57C65C9E-53E7-214C-9B4E-A75A6BAFD92C}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10922,7 +10781,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3A1AE775-B4ED-A64C-BD77-A5AB13F6CA86}" type="CELLRANGE">
+                    <a:fld id="{EF06EAB2-1839-254D-96EF-F8136CCAA2F7}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10955,7 +10814,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4DE75E94-67D3-4745-91C2-5373451EA48E}" type="CELLRANGE">
+                    <a:fld id="{979CD130-484D-3E42-A45D-BFE80C60036F}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10988,7 +10847,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9ADACC2B-2738-254A-B475-804A1CEA0A21}" type="CELLRANGE">
+                    <a:fld id="{D3DF324B-CCEE-194C-A4FE-04DAD03D5DC6}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11021,7 +10880,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3B1C47EA-C119-6F45-9260-BF9202418C6B}" type="CELLRANGE">
+                    <a:fld id="{B94F8B86-C9CE-A34E-9F13-38BD140BBF84}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11054,7 +10913,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{231B6B13-0850-514E-B08C-AD3269C2F239}" type="CELLRANGE">
+                    <a:fld id="{B59B36B1-A174-C14B-810D-C9DD7520EF3E}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11087,7 +10946,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{24B42B0A-2CD3-4C4A-A9E1-9E1C6CB3144A}" type="CELLRANGE">
+                    <a:fld id="{306A1F97-6AE4-524E-8B51-5FC9A145E936}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11120,7 +10979,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7D0ACB35-04ED-AB42-80E4-DBCA769207FC}" type="CELLRANGE">
+                    <a:fld id="{315431B2-3F45-FD4A-AE90-281136B015DD}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11153,7 +11012,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{02A46C82-551F-F44C-9094-77B3012D858A}" type="CELLRANGE">
+                    <a:fld id="{0C71526E-ACB8-9D4F-B550-C894F25DC246}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11186,7 +11045,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D3F09C22-4779-1148-8FD3-DC45C3A16608}" type="CELLRANGE">
+                    <a:fld id="{33E8B2AB-68F9-694F-B831-F78DE545AB94}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11219,7 +11078,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7297E657-A69F-F646-9193-CB65727A8E10}" type="CELLRANGE">
+                    <a:fld id="{AF806AF9-FA49-3F41-8951-B6DE13865EC5}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11252,7 +11111,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1CB1860D-DC50-7B45-AC9E-3D1BA3FA7738}" type="CELLRANGE">
+                    <a:fld id="{0AAFE016-D480-564A-85D7-6115177D9BD5}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11285,7 +11144,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{700C17AD-00D4-CB4B-81E9-17493D5A990B}" type="CELLRANGE">
+                    <a:fld id="{E481CE4A-810C-3740-AD45-91E3A64D8E31}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11318,7 +11177,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3325C4AC-8055-DC4F-8995-172E66E96DBF}" type="CELLRANGE">
+                    <a:fld id="{A4DF61A5-2B1E-134C-A6FA-6CA141392D10}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11351,7 +11210,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4294E49B-4230-014F-A504-5C893DCC4C43}" type="CELLRANGE">
+                    <a:fld id="{E3336B07-892B-7A4E-861C-55A80D76DD09}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11384,7 +11243,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C435C52F-DF49-7F4C-9081-032A2F9A710F}" type="CELLRANGE">
+                    <a:fld id="{5EB9335B-44AD-2142-90E4-2E2FF3BD29A3}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11417,7 +11276,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D29ECF60-DD47-DC4B-987E-6B25555DB789}" type="CELLRANGE">
+                    <a:fld id="{29870FF3-FFBA-434D-B681-53905F52555F}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11450,7 +11309,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4F28C34D-C59B-824C-A481-816AD799698A}" type="CELLRANGE">
+                    <a:fld id="{1CA02D88-B43E-A244-8255-887170E457D9}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11483,7 +11342,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D1799DC6-4010-6247-A733-B5EC7DEB5ACE}" type="CELLRANGE">
+                    <a:fld id="{D17DAC72-AE73-3B4F-B468-9730BA9E12B4}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11516,7 +11375,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E0C18E9B-5716-0A46-A107-4D83C555FC9D}" type="CELLRANGE">
+                    <a:fld id="{7D001231-087E-324E-BCFD-97B2B3BB88E3}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11549,7 +11408,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2040A72A-90F1-6843-B254-472DDD6AC79B}" type="CELLRANGE">
+                    <a:fld id="{0330FE96-805B-264C-B887-257289FA18BE}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11582,7 +11441,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F717A3DA-88BA-3F4A-B943-CD1A22766DD5}" type="CELLRANGE">
+                    <a:fld id="{5993A025-D7A7-0542-9361-6BDF50B61914}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11615,7 +11474,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B0D88489-2761-3E49-B28C-0752FE3ED938}" type="CELLRANGE">
+                    <a:fld id="{91A3AE09-2E11-324A-AAA4-745E865E8C73}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11648,7 +11507,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{70C500DC-DAF4-B149-82B6-838B889B6952}" type="CELLRANGE">
+                    <a:fld id="{BB0DECE6-4FEB-C946-9A0E-D5DAF78BF864}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11681,7 +11540,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{78178AED-ED4E-DA4A-A0BF-2313F88E83D6}" type="CELLRANGE">
+                    <a:fld id="{F9DF0EB3-127F-824E-B023-94398E94881E}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11714,7 +11573,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FECE739C-6DCD-9541-93D4-7E09ABD6034F}" type="CELLRANGE">
+                    <a:fld id="{09BAF714-C012-7F4E-BC45-120ECF7899B1}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11747,7 +11606,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{30A7AFF6-9FC3-794C-B78E-CD776F24018E}" type="CELLRANGE">
+                    <a:fld id="{29BB2DA6-1681-964D-9EBF-536F51D6AE9D}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11780,7 +11639,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A91F8608-3319-184B-982E-7724DFD1988C}" type="CELLRANGE">
+                    <a:fld id="{79F4EEF1-5C67-6D40-B053-54E1536B1A40}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11813,7 +11672,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{017B8CBD-BEC6-2444-9286-9D587181099F}" type="CELLRANGE">
+                    <a:fld id="{5D30E5BE-C949-AC4B-B642-40598B12C2B8}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11846,7 +11705,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0E045BE5-C9DC-0B4C-A7C1-BAC61FC27E97}" type="CELLRANGE">
+                    <a:fld id="{7DD98576-7253-8049-8F5F-6E821FD6B62B}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11879,7 +11738,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C5FAB416-B153-8C42-8115-B29530D03604}" type="CELLRANGE">
+                    <a:fld id="{E44E967A-C8E1-164B-AC83-57557ADCB545}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11912,7 +11771,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4293D00D-99A6-D441-B388-5CEE164DF6CC}" type="CELLRANGE">
+                    <a:fld id="{C3FFCA9E-DA56-E644-83C0-1AA4922D820D}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11945,7 +11804,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{59821228-C28B-504B-8AB1-F8403008B34A}" type="CELLRANGE">
+                    <a:fld id="{EB31250F-33AC-B246-9FD8-02BA78C86F3F}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11978,7 +11837,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{023A9010-BFE3-AB4C-989E-3598BE88FD00}" type="CELLRANGE">
+                    <a:fld id="{2B2F1CE7-753D-8F4F-89C6-69EE90BF32AC}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13016,7 +12875,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B257E246-C29B-404D-8AE3-853367D96F47}" type="CELLRANGE">
+                    <a:fld id="{D78F3574-5020-8144-9485-8871203C8191}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13049,7 +12908,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4B4C7B0E-EE61-D943-A0E7-473E1DFE741B}" type="CELLRANGE">
+                    <a:fld id="{32DE00E9-BC4D-EA4D-86F7-E21CE551D9D4}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13082,7 +12941,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{22CC9541-9497-8641-8E06-0959F51DDD9C}" type="CELLRANGE">
+                    <a:fld id="{9CD2BC81-1BC3-1C4B-8EFA-CDEBE51B92DD}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13115,7 +12974,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{29873030-C709-B748-8914-6645F3008BBC}" type="CELLRANGE">
+                    <a:fld id="{C0C1327D-AAF0-CB46-804C-499A83DCC94B}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13148,7 +13007,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5CDD1279-BCC2-8D4A-A3B1-9008295A1F3D}" type="CELLRANGE">
+                    <a:fld id="{B5D34600-1F22-3448-9BA6-07AC36D92336}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13181,7 +13040,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A1BED4B3-D91F-474C-AD3C-576B53033221}" type="CELLRANGE">
+                    <a:fld id="{A1B16CE5-673C-B34A-A3AB-99CB6EED4F5E}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13214,7 +13073,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CE8CF0BF-C5B7-224C-A9A3-149D88031B1E}" type="CELLRANGE">
+                    <a:fld id="{4387E8DD-E6F1-E548-BDEE-D0FFF979E7B4}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13247,7 +13106,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C32FCBCC-A06F-ED47-8FF1-F91E170AA396}" type="CELLRANGE">
+                    <a:fld id="{C9C84336-7C3B-564E-B48B-2AB7769DFE5C}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13280,7 +13139,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BAE3DBEB-BF75-FC4C-AD69-E5747B3E2E2A}" type="CELLRANGE">
+                    <a:fld id="{2E31C823-886F-F54F-89D2-98495C1E534B}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13313,7 +13172,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A655A655-1655-0E4D-A392-A48B9EEA2162}" type="CELLRANGE">
+                    <a:fld id="{DE0AF509-F033-024E-A4E2-30CAF6345B45}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13346,7 +13205,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EBFF380C-F63C-854E-86BB-33C2B5626278}" type="CELLRANGE">
+                    <a:fld id="{15F7B7FD-F0CD-BC4F-81AA-BDE128E09F10}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13379,7 +13238,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8A7ACFA6-52FC-0643-B2D0-914E670BA95D}" type="CELLRANGE">
+                    <a:fld id="{B1FF2AAD-CD7D-624B-9191-5F3DF346BFAB}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13412,7 +13271,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3F823962-C949-B143-9E13-91E067B6FC67}" type="CELLRANGE">
+                    <a:fld id="{797194E3-5C87-1944-A27F-DEBDBCCACD8B}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13445,7 +13304,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3B04198C-A81C-B446-8298-9DBE21C0DB40}" type="CELLRANGE">
+                    <a:fld id="{9B9A02F1-F642-FF4D-81AE-ED75D4C7DBE7}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13478,7 +13337,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DC4B1745-375A-D54F-B12D-93A34B7B83F5}" type="CELLRANGE">
+                    <a:fld id="{9D529017-8BE9-5247-ABC1-A77399FFD1B6}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13511,7 +13370,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EC21753F-3255-2B49-9A50-DB190DE092A8}" type="CELLRANGE">
+                    <a:fld id="{E45F5702-4C18-FE44-B5DD-ABB24E8040FF}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13544,7 +13403,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0542CE6E-6FD5-0D42-AC1E-DB4F21D14603}" type="CELLRANGE">
+                    <a:fld id="{2292F711-2811-9C4B-8D64-726FB42C8E7E}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13577,7 +13436,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CD737566-76C4-624B-9614-D55E4D3BF973}" type="CELLRANGE">
+                    <a:fld id="{EE13DAFE-22AB-954F-BAF9-A435A34BBD7F}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13610,7 +13469,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7C226648-B7E9-C347-92EC-5BD89A31F492}" type="CELLRANGE">
+                    <a:fld id="{65976132-F00D-EC4D-97A9-5FFC87A2B692}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13643,7 +13502,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B5AAB278-8B44-FB4C-AC4E-1FEFFF2EFE66}" type="CELLRANGE">
+                    <a:fld id="{AC687B52-B632-554F-80D8-7686BEF71596}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13676,7 +13535,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FD91CCCA-6117-CF4C-ABE7-81BBBDB3F958}" type="CELLRANGE">
+                    <a:fld id="{B223D205-59C8-0C44-85AA-5766D2E18AF6}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13709,7 +13568,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{23235455-E02D-CA4E-860A-C91D27CAD117}" type="CELLRANGE">
+                    <a:fld id="{EB1E8C89-B350-554C-A44E-4A8E27086744}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13742,7 +13601,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0E9105CF-63E2-DA43-9A5E-AE7A59514EA3}" type="CELLRANGE">
+                    <a:fld id="{9BA77C7D-9130-6446-BAF0-BFFA10C615DB}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13775,7 +13634,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{08F8288C-C992-4348-B399-32254EF285A8}" type="CELLRANGE">
+                    <a:fld id="{7537B783-0F77-3749-9CAF-4C49EE1FCB37}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13808,7 +13667,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CB90B282-9E92-B44E-B9FB-7F2E1CBFD16F}" type="CELLRANGE">
+                    <a:fld id="{2913EB78-876F-9B40-B31A-99E1012AC0BA}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13841,7 +13700,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4174405C-5F76-A94A-8A02-3B2385AF261D}" type="CELLRANGE">
+                    <a:fld id="{2655A36F-2C37-2A4E-9D35-AEC2F499CABA}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13874,7 +13733,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F79CD260-82CE-5A43-9B07-77AA23CD020F}" type="CELLRANGE">
+                    <a:fld id="{377C4748-7D46-2440-993B-5B6705559E89}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13907,7 +13766,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{220FA6D6-99DA-B545-865D-AF5F7E750978}" type="CELLRANGE">
+                    <a:fld id="{76E44B17-2244-8347-A084-915F5D35694B}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13940,7 +13799,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CD00CCE3-5C5E-5D43-92B9-337950E1C644}" type="CELLRANGE">
+                    <a:fld id="{22950290-2D85-7E4A-B972-01CB696C6B90}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13973,7 +13832,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CD4CD6EE-C57B-9C4C-AC36-1BEEFE6D9991}" type="CELLRANGE">
+                    <a:fld id="{7D17262D-883E-954B-B1B6-C1353BD888DF}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -14006,7 +13865,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CFACF625-7076-874F-9BFF-5AC3E3AE676E}" type="CELLRANGE">
+                    <a:fld id="{93B22B20-167E-6443-960E-5FA079FCFF62}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -14039,7 +13898,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A75D95C0-2E71-7746-AEED-0F44DDA5B3F1}" type="CELLRANGE">
+                    <a:fld id="{C0F3E88A-289C-2340-90FE-AF5D861EB7F6}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -14072,7 +13931,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{531C3C1A-3AFD-874A-A1F2-7C919F69C8F1}" type="CELLRANGE">
+                    <a:fld id="{BAE47B88-5B9D-0640-938F-5B1058D18783}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -14105,7 +13964,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B9C8C716-0974-0F41-9937-71F91FA6EAF4}" type="CELLRANGE">
+                    <a:fld id="{AB98A391-3F0D-D745-A5A5-FBF55C4BA74C}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -14138,7 +13997,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C3012855-EC2D-2A49-986C-D48A2D9726A7}" type="CELLRANGE">
+                    <a:fld id="{34DFADA5-C9B6-FC47-9D13-B1E74A7328EA}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -14171,7 +14030,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D26FF3FB-CD2A-AB49-8226-6462AF74D8C6}" type="CELLRANGE">
+                    <a:fld id="{1536F8EF-DD63-624F-91AA-F98BC2CCCA06}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -14204,7 +14063,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9BBD1F6E-168F-4243-B69E-C31359A4A9A9}" type="CELLRANGE">
+                    <a:fld id="{B15B325B-68E4-A442-B434-FCD39D2D2716}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -14237,7 +14096,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8056F5F8-6482-F64B-9807-7DAAE9DD1AE3}" type="CELLRANGE">
+                    <a:fld id="{C4B0A380-CCE8-EB45-8A10-ACD3ADB5355D}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -14270,7 +14129,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E9F11E01-B36A-ED4F-B96F-DCE8E3C5C195}" type="CELLRANGE">
+                    <a:fld id="{DA541FA6-197B-3E41-972A-61BB7C3F79CE}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -14303,7 +14162,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{47D0588B-DB3C-364B-BC0E-FC7AE50ED7C8}" type="CELLRANGE">
+                    <a:fld id="{5EA9563D-8FE7-844C-BCF1-FD682BA8FC77}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -14336,7 +14195,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8F942D46-0520-914F-9C80-BE62398A0AEE}" type="CELLRANGE">
+                    <a:fld id="{051FAD65-1FB1-4B4B-BCB2-1C67DBD5DEF6}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -14369,7 +14228,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{40164FCB-43A0-FD4D-9F1E-34810CFF2789}" type="CELLRANGE">
+                    <a:fld id="{8231BAED-7B40-4041-B291-202EA3BE656B}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -14402,7 +14261,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{62095201-FC1F-7346-BD9A-71D00DC7AF91}" type="CELLRANGE">
+                    <a:fld id="{00F04A0A-9CF9-9642-BA75-9FA2541B51EE}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -14435,7 +14294,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6DD2126C-41ED-674C-9615-278F000AF009}" type="CELLRANGE">
+                    <a:fld id="{70C30B0A-68D2-B442-A119-324CD7F31B6D}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -14468,7 +14327,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{005AC20A-77EA-524B-8F3E-219A657C19A0}" type="CELLRANGE">
+                    <a:fld id="{43B84547-1CE8-B741-8ABA-40BE9C765ED7}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -14501,7 +14360,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CDAE46F1-E21E-E147-94C7-4211DF471500}" type="CELLRANGE">
+                    <a:fld id="{E4DD8E4B-633F-3F47-88B8-270758AA904C}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -14534,7 +14393,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{70BA7D28-1B41-0344-9C46-A10EE56E168C}" type="CELLRANGE">
+                    <a:fld id="{2967F7EE-2747-B143-A0FC-0B5329651B92}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -14567,7 +14426,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2A5BF7AB-17CE-E140-BC9F-A03173B9A120}" type="CELLRANGE">
+                    <a:fld id="{F6E26CC4-5202-B849-9AB1-31B7090EAFD4}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -14600,7 +14459,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{19560BD1-3494-9C40-8F48-3B56E79FF629}" type="CELLRANGE">
+                    <a:fld id="{A2AF37C1-0626-7845-BB96-CDB444F28ACF}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -14633,7 +14492,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FF5786FB-4639-3740-86DB-DD09BE5BE79C}" type="CELLRANGE">
+                    <a:fld id="{5668C4C0-978C-D947-B8F2-E8776ED471B2}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -14666,7 +14525,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AB05083E-D9AD-C44F-9630-4AF0F0A2A280}" type="CELLRANGE">
+                    <a:fld id="{4539189C-0F4E-4C41-967C-D14E67FD2E0F}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -14699,7 +14558,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{11730657-79FD-CA40-AD78-CACEFA3E1040}" type="CELLRANGE">
+                    <a:fld id="{CBF832EE-5B6A-F54F-B84C-F106C94F1541}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -14732,7 +14591,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{495CB112-8CE5-B344-A2E2-ACC2AA39E8E8}" type="CELLRANGE">
+                    <a:fld id="{A4A5CF9D-3DBD-4046-A38D-3DBB190534CF}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -14765,7 +14624,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5F279E88-1B48-9746-864A-780E7B009D36}" type="CELLRANGE">
+                    <a:fld id="{39D3D92A-8F26-4447-96FF-7FC983229F6F}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -14798,7 +14657,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{232EB5C6-9E85-2E47-92B7-6C265B6779E3}" type="CELLRANGE">
+                    <a:fld id="{5D19BEE3-04A0-C34F-80C0-23CB96389629}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -14831,7 +14690,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{24B66C0E-F59E-FF48-B99E-98755D1E1183}" type="CELLRANGE">
+                    <a:fld id="{93124AA7-2515-3142-825F-AC5EA71360E8}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -14864,7 +14723,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CB929465-378A-1047-831B-36B286BFAF8D}" type="CELLRANGE">
+                    <a:fld id="{0778D4B9-B9B3-A245-9A42-557AECD20C1F}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -14897,7 +14756,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{749C9385-6C50-4545-A228-EE79AFC74BD7}" type="CELLRANGE">
+                    <a:fld id="{425F364D-F9A2-D649-8E77-5B68DC74F249}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -14930,7 +14789,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1C10C03E-A1CB-8F45-B0B5-B98778E95B56}" type="CELLRANGE">
+                    <a:fld id="{F1E22957-7B16-2443-B879-F5B131E55326}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -14963,7 +14822,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BC7FA494-2492-6044-9CA5-E9A226B0F088}" type="CELLRANGE">
+                    <a:fld id="{76AF44DB-DE19-6C49-841B-78A39A320638}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -14996,7 +14855,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{82EB8907-7835-D243-A92A-C0D5F9779835}" type="CELLRANGE">
+                    <a:fld id="{38814680-EF7C-4C43-BAC0-DE33E67909D2}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16003,7 +15862,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FEF780DD-62DB-3C42-8B11-8C264601BCF8}" type="CELLRANGE">
+                    <a:fld id="{252DA042-0EEA-C64F-B6D8-0187EB9EEB18}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16036,7 +15895,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9C8823D4-650E-4644-9FDD-254124896CBA}" type="CELLRANGE">
+                    <a:fld id="{F3E86E3D-6911-3143-89B7-36D29F335515}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16069,7 +15928,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EA95F673-7586-4A4B-9AFE-443734913486}" type="CELLRANGE">
+                    <a:fld id="{AFD5A4E0-C220-CD40-AFA9-E57E49FDE16A}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16102,7 +15961,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5D8664AF-8562-2649-843A-0B1A883E1200}" type="CELLRANGE">
+                    <a:fld id="{315E69D5-D6CF-4E48-8B24-E488802EFB7B}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16135,7 +15994,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2D1D5B87-252A-B041-9664-685AB5065017}" type="CELLRANGE">
+                    <a:fld id="{59E12FCC-C0B5-3842-BB26-D0B9551D4005}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16168,7 +16027,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D1B8B081-39D8-C846-B87A-12AA80AE6772}" type="CELLRANGE">
+                    <a:fld id="{A9E0F4C7-4022-A24A-9FFD-7DE567EC5E48}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16201,7 +16060,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FD8E0740-60ED-ED4B-93BE-AE72127DE0EE}" type="CELLRANGE">
+                    <a:fld id="{D588B642-1C88-0843-8727-DF5094CB5E4E}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16234,7 +16093,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{187DF3FF-7CC3-5B4F-BD57-508B4BD8219A}" type="CELLRANGE">
+                    <a:fld id="{2CF1A5FD-1BB2-204F-8BD4-4C167A7B44D5}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16267,7 +16126,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{374B6212-03B1-094F-92B8-4B3C3B706559}" type="CELLRANGE">
+                    <a:fld id="{0B7C2866-B381-7E40-94A8-5720982CA037}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16300,7 +16159,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2CC229FB-AC64-B142-893B-373798A9134B}" type="CELLRANGE">
+                    <a:fld id="{6780C86C-5E62-024C-9C4A-397382459C2B}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16333,7 +16192,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{289BAB82-B33D-F249-A4F3-5CD9139FC35A}" type="CELLRANGE">
+                    <a:fld id="{044B422B-5D63-A547-A48A-95B2A92B11FA}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16366,7 +16225,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E6DCEC28-0647-A548-882F-F065C9A01FB9}" type="CELLRANGE">
+                    <a:fld id="{BFC4135E-205E-714A-A3CD-5D8304517827}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16399,7 +16258,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{862BA102-DB7E-4D49-A5A9-6ABBEA5140D6}" type="CELLRANGE">
+                    <a:fld id="{98AA670F-AD4F-1547-A5CB-64D18C193EC6}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16432,7 +16291,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AAD53782-A8FD-D049-A138-244B7610F783}" type="CELLRANGE">
+                    <a:fld id="{FD8E4280-C6A9-1B4D-8379-3FB82893C819}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16465,7 +16324,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{29CAD8A8-7FCC-5F4C-9DC3-0E8C6172623D}" type="CELLRANGE">
+                    <a:fld id="{A72BAB44-F0BE-FA41-8F8D-FE9659889083}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16498,7 +16357,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{32C8402B-A723-AA44-A223-9E4803A04F29}" type="CELLRANGE">
+                    <a:fld id="{EAF39937-165A-B740-A046-CD1EECCD3051}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16531,7 +16390,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7615B3BB-23C0-384C-A01B-0B3BF2533B99}" type="CELLRANGE">
+                    <a:fld id="{C7C8D45B-0813-004A-B923-7F77785B26E2}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16564,7 +16423,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{79910D85-09C2-0149-A3B6-0B3DF278B3C3}" type="CELLRANGE">
+                    <a:fld id="{67155F28-D721-0843-9200-7F7D9506C9FB}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16597,7 +16456,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FA50071D-66F3-AB49-A55D-E172DBD9DE2D}" type="CELLRANGE">
+                    <a:fld id="{44236840-92B2-6149-B0C8-7855E914C392}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16630,7 +16489,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{891DE284-8FF0-0949-82CF-C4083BD80437}" type="CELLRANGE">
+                    <a:fld id="{CBA58BC0-B5B5-3642-9962-EF0884AF5E75}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16663,7 +16522,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EF180FB0-E5BB-B24B-9450-A42E1CE956F1}" type="CELLRANGE">
+                    <a:fld id="{B6C2568D-0C89-614D-A03A-701539B1B3CD}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16696,7 +16555,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2863A4C5-0EE0-8C41-9449-FEB108574F69}" type="CELLRANGE">
+                    <a:fld id="{64A17128-053E-9546-BD03-717814A0AEA6}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16729,7 +16588,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{998209D9-4649-CC4F-BD14-B1176936EE99}" type="CELLRANGE">
+                    <a:fld id="{4BEC1B76-E839-244A-A313-F3664306F1A4}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16762,7 +16621,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{443AEDC2-3FDA-244F-8724-06D907CF1C5A}" type="CELLRANGE">
+                    <a:fld id="{FF70034F-5713-B044-B29D-0EFF759E729A}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16795,7 +16654,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2D3019E7-2E90-404B-888D-55CECD660250}" type="CELLRANGE">
+                    <a:fld id="{BD8865C9-E6FC-3542-B70F-EB2125151E64}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16828,7 +16687,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0F1D70FC-70A6-D444-BC6A-DEDC0072B032}" type="CELLRANGE">
+                    <a:fld id="{D9EFD626-0CF4-FD4A-A430-F781D88F00E5}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16861,7 +16720,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{25A4C9CC-CACF-7242-A532-9F70EB551105}" type="CELLRANGE">
+                    <a:fld id="{C8347A66-91C9-AA4A-B26E-FCF20F7BCA7C}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16894,7 +16753,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{48912F2E-B5A3-784F-AB36-70BDA5968B6C}" type="CELLRANGE">
+                    <a:fld id="{BD0ABCAF-CE60-124D-A7D3-C08C7F42428C}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16927,7 +16786,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D7B0E617-4438-0446-B208-44CE1CB541E3}" type="CELLRANGE">
+                    <a:fld id="{6649D930-43BB-2842-AC74-FF0C6349E3AE}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16960,7 +16819,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{31B7860A-419D-284D-A1AB-9480FC9B0BAA}" type="CELLRANGE">
+                    <a:fld id="{7A259CED-8FE2-B246-B452-8102A92DA2CE}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16993,7 +16852,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E88F6DAC-EA56-044A-A8EC-8C320A05EE5B}" type="CELLRANGE">
+                    <a:fld id="{A26DFE9F-E1F2-8943-8AAD-927A0142E6E3}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -17026,7 +16885,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FD2D3049-2189-0D44-8510-DE26CF1FD25F}" type="CELLRANGE">
+                    <a:fld id="{25BC3C48-5260-154B-903A-50584AF2005F}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -17059,7 +16918,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{263DF78E-5F61-9942-A1D3-FFECE9E5ACCE}" type="CELLRANGE">
+                    <a:fld id="{99119A8F-89EF-5B4F-B7AC-BE159EAAEE87}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -17092,7 +16951,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{611E5BCF-7561-3A47-8C3A-1ECC471049A2}" type="CELLRANGE">
+                    <a:fld id="{D3DC8CB7-4FC0-4D4B-A921-7044E6BE3AEB}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -17125,7 +16984,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EDB13E6F-DF2D-A34A-AED5-C9F1EDB1CF60}" type="CELLRANGE">
+                    <a:fld id="{9FEF4337-9590-EC43-9705-96E2254B9AB5}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -17158,7 +17017,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D7D82A63-CC86-AB42-BD7C-929D3B7A8890}" type="CELLRANGE">
+                    <a:fld id="{D31AEBDE-FB19-3641-89A5-DD5D10075FFF}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -17191,7 +17050,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9F2CC7CB-CC96-CD42-9E84-322F54F7A429}" type="CELLRANGE">
+                    <a:fld id="{0798B8E4-76AA-9C42-A0C6-7CFD1BE62F0C}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -17224,7 +17083,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8FBFA7F3-ED88-A64E-A973-16A11BAAE2C0}" type="CELLRANGE">
+                    <a:fld id="{35F3DF50-284C-9346-A197-32BAD92F30C8}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -17257,7 +17116,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{75AD8B1F-A7A4-224C-B805-60816B0E0544}" type="CELLRANGE">
+                    <a:fld id="{6B809512-2F5A-4741-9121-DEC0CC0A432E}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -17290,7 +17149,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D681147C-634E-AF4B-860F-942B2B059BCB}" type="CELLRANGE">
+                    <a:fld id="{F82A2E46-CC04-3D4E-8533-6D257ED0D62C}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -17323,7 +17182,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{515BB6CC-27A0-CB46-8ACA-EFE1CFEA1DDA}" type="CELLRANGE">
+                    <a:fld id="{A8971502-CAA4-554B-8CFE-A2DBFF8A5496}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -17356,7 +17215,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DD38C26E-CFF5-5748-8CA0-4AB8E2EFEDB2}" type="CELLRANGE">
+                    <a:fld id="{DA42A018-7E7E-6144-A247-597866BDF964}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -17389,7 +17248,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FF51EF75-DEA2-AD48-8AA3-544F29881FA0}" type="CELLRANGE">
+                    <a:fld id="{9FFEE1C5-400D-BF4F-A2BB-9C5D29F89635}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -17422,7 +17281,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{66B64249-DFD0-8547-B4AC-90D098986EAB}" type="CELLRANGE">
+                    <a:fld id="{7E103434-A357-6E46-88A9-D7E8CC68C62F}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -17455,7 +17314,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7AD6CC2B-0D9C-F842-9CD8-E9D299D8B14F}" type="CELLRANGE">
+                    <a:fld id="{B77E37EF-7B52-1947-81CB-724975B65860}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -17488,7 +17347,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F55FD8A8-0237-2744-973F-68C32E053844}" type="CELLRANGE">
+                    <a:fld id="{39112BD5-038A-D449-9F2A-E05707FA4976}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -17521,7 +17380,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{09F2AD09-69F3-174B-AF10-B85C657FBF05}" type="CELLRANGE">
+                    <a:fld id="{5DA8816C-E981-D24E-8F2C-18CA710B081A}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -17554,7 +17413,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{38BF3079-833D-2B46-B76C-EF0191C06FB8}" type="CELLRANGE">
+                    <a:fld id="{A0B41FA5-E683-9E45-B1B6-63E3A998EC3E}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -17587,7 +17446,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B032D1A0-4A3E-4E48-85E9-0C323B4EE167}" type="CELLRANGE">
+                    <a:fld id="{1839479D-508A-5E43-8331-2C0A140295A5}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -17620,7 +17479,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5283BCF1-B45E-9242-94C3-B579B95AA32F}" type="CELLRANGE">
+                    <a:fld id="{B06D49C0-3292-6845-B8CE-B1F68906FF96}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -17653,7 +17512,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D3BEB16E-0431-6C4E-B148-DDD6B754F70F}" type="CELLRANGE">
+                    <a:fld id="{AA405ED5-A0D2-A845-8D59-877397303719}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -17686,7 +17545,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{53F0BF63-D1C7-E04E-9CCD-44B7DEEBF8E3}" type="CELLRANGE">
+                    <a:fld id="{64A9A4A2-1AF0-7B40-BF39-A260E379FF09}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -17719,7 +17578,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BF178264-5417-7F4A-B545-8D85AB98592F}" type="CELLRANGE">
+                    <a:fld id="{F8B3EE14-E32C-C643-BD78-33194D5B10A8}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -17752,7 +17611,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D1FD0EA3-528E-9045-9C1B-487BF1B86EC6}" type="CELLRANGE">
+                    <a:fld id="{52C2A093-CF91-404E-B91C-121965D51333}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -17785,7 +17644,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D4A5697D-96A8-244F-A7F3-F95A871587E3}" type="CELLRANGE">
+                    <a:fld id="{E996961A-1347-2C4C-B3DF-BC6EE3BB6A3F}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -17818,7 +17677,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{42ED223C-8380-094C-A943-AACE8AC33E22}" type="CELLRANGE">
+                    <a:fld id="{4E5D9E18-CE07-BB4B-BEC7-4F30809A8820}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -17851,7 +17710,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A0FF2D52-59AC-824C-B287-86AA45955C6A}" type="CELLRANGE">
+                    <a:fld id="{468B869F-D4D6-374E-AFC7-512545576A7D}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -17884,7 +17743,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{65F17C50-DFEB-664F-BE73-DF0A75C6BC7C}" type="CELLRANGE">
+                    <a:fld id="{CC5EFF60-7106-2640-A37B-EB3BCD35B53A}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -17917,7 +17776,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{556C72C6-979A-A345-BF41-238126175181}" type="CELLRANGE">
+                    <a:fld id="{5DE2270D-6F0C-6F42-A0A5-D9A8BCD21593}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -17950,7 +17809,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7C66AEB0-17FC-0F45-B84F-697F7A9EA105}" type="CELLRANGE">
+                    <a:fld id="{7CC50C4C-D773-C749-A791-FA35D564F063}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -17983,7 +17842,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D75BD17F-6359-6446-BADE-7612004DB8B9}" type="CELLRANGE">
+                    <a:fld id="{8AEB9E2D-95CC-9B4F-94B5-E0D602963C13}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -18968,7 +18827,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AD4536C4-EBCF-E745-9034-14C040CA4D8D}" type="CELLRANGE">
+                    <a:fld id="{D4BF8A76-6952-ED4F-A4D2-68418064A8BF}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19001,7 +18860,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{13707CC8-8F4A-5F46-950D-95B11EA9D908}" type="CELLRANGE">
+                    <a:fld id="{C121D75B-3CFE-0044-A660-BEB757BA3D8E}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19034,7 +18893,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AF071AD0-89B7-884A-A693-D30C8EB4C448}" type="CELLRANGE">
+                    <a:fld id="{5573DD70-32C7-784B-9667-84E326DB339B}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19067,7 +18926,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{392E1781-5D22-A644-BC19-E88695B586C8}" type="CELLRANGE">
+                    <a:fld id="{AFF6E373-D6CC-8844-A446-2F98BB8AA33E}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19100,7 +18959,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EF609506-AB32-234B-9F13-B90A749734BC}" type="CELLRANGE">
+                    <a:fld id="{3F919766-B993-2E4E-939C-A4D57E44E75E}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19133,7 +18992,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7032207A-8B8D-104E-9230-C0986CE984C7}" type="CELLRANGE">
+                    <a:fld id="{399808A5-5AA7-B846-BC57-08FBB1A02626}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19166,7 +19025,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A8AF0B0D-A6B4-8D4C-94E5-F10A874D03E8}" type="CELLRANGE">
+                    <a:fld id="{0975A2DD-B3FD-5A4A-B598-7DCE11CEC347}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19199,7 +19058,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{64D4A799-665B-9D46-B617-C30869E3BCCC}" type="CELLRANGE">
+                    <a:fld id="{4EB31919-0070-3245-9B72-D19081B33940}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19232,7 +19091,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{33EA4E5F-C1FB-CD41-8E42-6E3D312370DD}" type="CELLRANGE">
+                    <a:fld id="{3D01AF08-F674-BD43-9C21-1051068D1FB0}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19265,7 +19124,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A192E6C6-6D1C-6E48-9F1B-6334739ACAED}" type="CELLRANGE">
+                    <a:fld id="{7F1E8942-BC3B-5845-AE8B-1BC7AF339DB9}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19298,7 +19157,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5CC9621A-DD47-0B45-B184-9EBA8D56BC71}" type="CELLRANGE">
+                    <a:fld id="{1DDD8D46-3EA4-D647-A8F0-2B3A6A8C4C63}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19331,7 +19190,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1500BDCE-A0FA-AD4A-8A37-EA0A5194A924}" type="CELLRANGE">
+                    <a:fld id="{6B19808D-FDC8-CD4D-9096-B66D1F04DE0E}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19364,7 +19223,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7C637087-E2AA-A94B-A9AF-C8536A904C79}" type="CELLRANGE">
+                    <a:fld id="{E53F7EAB-595A-CF45-9F8D-1274F87C8BAE}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19397,7 +19256,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DB4937E0-49E8-BC4E-A4FE-053C99B317A0}" type="CELLRANGE">
+                    <a:fld id="{1FC7FCB2-E3FE-9047-A2BD-7582A95B5D01}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19430,7 +19289,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B597414A-7C5E-BA45-98FC-0E4FEC2F8EFB}" type="CELLRANGE">
+                    <a:fld id="{B72B41FE-57FD-9A42-A8B1-F9E537DA6FC2}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19463,7 +19322,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4D0217C1-9750-CD46-B880-7301367489F0}" type="CELLRANGE">
+                    <a:fld id="{B26881BD-6006-2047-B90B-AF933706E784}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19496,7 +19355,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E5F09B6B-B564-F241-97AC-E42AE269F904}" type="CELLRANGE">
+                    <a:fld id="{41FAF8FA-769C-7F49-B041-F15379218AE9}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19529,7 +19388,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{389D342F-968E-8F4D-B85B-DCA8AE369014}" type="CELLRANGE">
+                    <a:fld id="{BD502E3A-CD4B-F04D-BD05-B0C09ADCCF8B}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19562,7 +19421,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{80AB4AB0-664D-9F49-9525-36AF58BE4244}" type="CELLRANGE">
+                    <a:fld id="{76C28486-3C40-D345-8BD5-63CE29C115E8}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19595,7 +19454,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{26BAABDC-1D7B-AE47-929B-901C11276A73}" type="CELLRANGE">
+                    <a:fld id="{AD08FA31-B1B5-4A4A-AA77-6940A4A3EC28}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19628,7 +19487,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C4C1780F-CCBC-9448-A406-1073B12D2A33}" type="CELLRANGE">
+                    <a:fld id="{AADB7024-353E-F64F-800A-B3CB891C3BF5}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19661,7 +19520,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{85A50ED8-75E4-F34D-BEA7-817CC1E622B7}" type="CELLRANGE">
+                    <a:fld id="{108D9F40-9B07-A64B-8903-D4DADCBAA286}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19694,7 +19553,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{980647E5-81AE-A849-BB0A-B950290ED087}" type="CELLRANGE">
+                    <a:fld id="{871EA5AA-541D-844D-BEE5-B6575D834935}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19727,7 +19586,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{36C4030F-67D2-F74F-89E6-B78A996B741B}" type="CELLRANGE">
+                    <a:fld id="{29321414-FFB2-4D41-A5EA-C40213B8A445}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19760,7 +19619,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C5676A5E-D537-AE47-9D5D-10EEB277281A}" type="CELLRANGE">
+                    <a:fld id="{A6D08340-3A74-3446-94A0-8DF690BFEDC3}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19793,7 +19652,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{70B4FB54-0EA9-E449-A16D-FB0592E30E88}" type="CELLRANGE">
+                    <a:fld id="{FA6BE134-190F-7641-BC1D-11AB4FCF7944}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19826,7 +19685,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4FE6B70E-8F82-0346-8648-CA97B214B324}" type="CELLRANGE">
+                    <a:fld id="{DA966284-15E3-894A-947A-DB25D07AD944}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19859,7 +19718,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{22E4ADE0-D681-9347-AA47-E1DDB6A4DA52}" type="CELLRANGE">
+                    <a:fld id="{C6C77E34-F797-AD44-9D52-BA45B8AA168F}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19892,7 +19751,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DDA9D9AA-77E4-ED44-9F4E-8BB003563D57}" type="CELLRANGE">
+                    <a:fld id="{9D1253B8-3075-814B-BE4E-84B3C179475C}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19925,7 +19784,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B4A11463-6A63-8A4C-BE4C-681E83E4196D}" type="CELLRANGE">
+                    <a:fld id="{0A0B6718-116D-014D-8DEB-26779A20BF5B}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19958,7 +19817,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B85388C8-9D53-A34D-BEF3-02F232B682BA}" type="CELLRANGE">
+                    <a:fld id="{63A805B2-5237-D249-B7DC-6C20BE900512}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -19991,7 +19850,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0CAB712C-9129-C34D-B935-C4A2AE552021}" type="CELLRANGE">
+                    <a:fld id="{42084BE1-CE5A-3940-8695-40A5F4B88430}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -20024,7 +19883,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2EC99C63-0261-C343-A45C-95942B62FA1D}" type="CELLRANGE">
+                    <a:fld id="{41412C87-BFEE-F64E-9283-2A415F3EC88D}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -20057,7 +19916,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C76D8B06-BCA7-014F-8F58-A70BEF5E7273}" type="CELLRANGE">
+                    <a:fld id="{51714DBB-0AC0-8448-8DAD-A77CB86DF0B6}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -20090,7 +19949,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{45C025E1-5240-B943-997C-05F13AEB7660}" type="CELLRANGE">
+                    <a:fld id="{2728973D-B147-EC4C-9026-C5709914AF92}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -20123,7 +19982,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4FA41264-290D-0844-B6F3-F7F9D683CC32}" type="CELLRANGE">
+                    <a:fld id="{77B9DAB7-FE74-C34D-BDE9-F883BF7036CF}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -20156,7 +20015,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F2EF47E5-B064-444E-9C8B-2560B13398E7}" type="CELLRANGE">
+                    <a:fld id="{85087EBC-1DA0-A042-8E82-676068D378D2}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -20189,7 +20048,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7D76E21D-BB2F-F34D-9279-FEE5A9181518}" type="CELLRANGE">
+                    <a:fld id="{5BC9A818-3EEF-7F42-BAF3-4041BD0B6559}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -20222,7 +20081,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C3BE3996-4EE2-AA42-93C2-B165FD641DDC}" type="CELLRANGE">
+                    <a:fld id="{988A96C0-1932-5D49-928F-E4749707FCBB}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -20255,7 +20114,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B6D06365-DD8F-264E-A99B-5DFDAC1A0E91}" type="CELLRANGE">
+                    <a:fld id="{3075E213-9B5D-4A4E-91EA-CAEE2845581B}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -20288,7 +20147,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C6C6C218-6521-B14E-B670-036DA20791A1}" type="CELLRANGE">
+                    <a:fld id="{141E5E81-3730-FE4E-974F-C454BBC3390D}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -20321,7 +20180,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{672FCEEF-EDE5-1349-893E-FCC0EEF2F2BA}" type="CELLRANGE">
+                    <a:fld id="{CC7A62FF-E93B-9E4C-90F3-299263D81D22}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -20354,7 +20213,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D761EB5F-16D0-D145-A747-CFFCFB1A3389}" type="CELLRANGE">
+                    <a:fld id="{25A26A3D-37D9-C04E-B690-613CA4B34E43}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -20387,7 +20246,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{11721A13-1006-F54D-99C2-FB163775E9BB}" type="CELLRANGE">
+                    <a:fld id="{FEF99CB9-86A2-644C-AA0A-93BEA189B36B}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -20420,7 +20279,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C8DC8A2D-ED4D-5D45-967D-DA66679ADDA6}" type="CELLRANGE">
+                    <a:fld id="{AA3F1795-AE58-A44A-8820-47E503991CD9}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -20453,7 +20312,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{51CA5888-A884-B644-93D5-DFC281CE47D7}" type="CELLRANGE">
+                    <a:fld id="{799E21F7-866E-974E-A198-FDC2F96C44FF}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -20486,7 +20345,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D0953A96-970B-2544-9749-EB81DB020402}" type="CELLRANGE">
+                    <a:fld id="{F64222F6-3705-7246-AE8C-16712055CEFA}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -20519,7 +20378,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{52E7DCCB-D399-AB46-8B6E-FB90DDDCAE54}" type="CELLRANGE">
+                    <a:fld id="{2C0D88D0-EA49-764B-B397-ADB01AB65A33}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -20552,7 +20411,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{61BE70E3-B83E-FC40-B247-C8C667F00CA2}" type="CELLRANGE">
+                    <a:fld id="{A5795D67-E4BD-A449-BC3E-4B6BBA40B384}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -20585,7 +20444,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FDFA7D14-4A1B-1443-BD3F-4006878B929F}" type="CELLRANGE">
+                    <a:fld id="{AC0F56E3-16EF-FB4E-92FC-BF76F8FFA784}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -20618,7 +20477,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3607C38D-7A7F-E246-8311-6130AFF4BFA0}" type="CELLRANGE">
+                    <a:fld id="{08C1975C-91FE-B74B-AD6E-50C62A7FEEDA}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -20651,7 +20510,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B72AC228-82D0-F24C-B451-7DF1C3DF9678}" type="CELLRANGE">
+                    <a:fld id="{694D516F-770A-424E-B571-52DA5976925A}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -20684,7 +20543,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{38DD7D9B-EC91-944F-94BE-2449AB084905}" type="CELLRANGE">
+                    <a:fld id="{C12A71CC-D7FF-B146-B8DB-51B3A1724D09}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -20717,7 +20576,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{03C7D28C-4EA3-6A43-AF89-5AA8DEC661BA}" type="CELLRANGE">
+                    <a:fld id="{7700203F-BA89-C849-829F-E53743955746}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -20750,7 +20609,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{68CE9283-D900-0B4C-A2E8-8AC04042CF02}" type="CELLRANGE">
+                    <a:fld id="{A1DA60CC-C713-EE44-9C6F-D2C56FC5D78B}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -20783,7 +20642,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1AC20D02-CC47-F84A-B7C4-DBCCF927C205}" type="CELLRANGE">
+                    <a:fld id="{04A70276-93F5-B848-9F21-B18D54C16E5F}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -20816,7 +20675,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{15FFE72F-E8C9-8F4A-8F2C-410B8734F740}" type="CELLRANGE">
+                    <a:fld id="{ADFA3F65-44F7-344E-8422-48C2D159DC72}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -20849,7 +20708,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0F1523C9-8B58-AD49-BDCE-3B732A9A0D90}" type="CELLRANGE">
+                    <a:fld id="{E18BED7F-6DCD-0649-90D7-AED85489722B}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -20882,7 +20741,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{448072DB-75E0-F943-9E62-59AA4681713D}" type="CELLRANGE">
+                    <a:fld id="{8670B94B-5341-1B4A-809C-CDB3988AD4B1}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -20915,7 +20774,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{21F4A119-BEFC-794F-9ABC-47FB74CE6497}" type="CELLRANGE">
+                    <a:fld id="{344C64E3-18E4-FB48-96E8-9E52C32816F9}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -20948,7 +20807,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8A0F5CF2-70BC-2A42-BEAB-E134FFE9057C}" type="CELLRANGE">
+                    <a:fld id="{D14D3B3A-2A5A-6D4B-A9BC-B63C4D3866EE}" type="CELLRANGE">
                       <a:rPr lang="es-MX"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -25753,7 +25612,7 @@
                   <a14:compatExt spid="_x0000_s1025"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9D57635-83DE-E882-E331-0AB263C18ED0}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -28621,7 +28480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4053C8FF-5711-3B4F-9AD2-AFA8CF4BACB3}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
@@ -28631,6 +28490,190 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D29C05AE-70A8-2B42-9F1B-DB98428C6E57}">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="C2">
+        <v>4.6299999999999996E-3</v>
+      </c>
+      <c r="D2">
+        <f>B2-0.122</f>
+        <v>0.11000000000000001</v>
+      </c>
+      <c r="E2">
+        <f>B2-0.187</f>
+        <v>4.5000000000000012E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>0.217</v>
+      </c>
+      <c r="C3">
+        <v>0.11</v>
+      </c>
+      <c r="D3">
+        <f>B3-0.0406</f>
+        <v>0.1764</v>
+      </c>
+      <c r="E3">
+        <f>B3-0.0757</f>
+        <v>0.14129999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="C4">
+        <v>6.9599999999999995E-2</v>
+      </c>
+      <c r="D4">
+        <f>B4-0.0521</f>
+        <v>0.23789999999999997</v>
+      </c>
+      <c r="E4">
+        <f>B4-0.109</f>
+        <v>0.18099999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>0.128</v>
+      </c>
+      <c r="C5">
+        <v>0.441</v>
+      </c>
+      <c r="D5">
+        <f>B5-0.00959</f>
+        <v>0.11841</v>
+      </c>
+      <c r="E5">
+        <f>B5-0.0516</f>
+        <v>7.6399999999999996E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>0.44700000000000001</v>
+      </c>
+      <c r="C6">
+        <v>7.0499999999999993E-2</v>
+      </c>
+      <c r="D6">
+        <f>B6-0.0518</f>
+        <v>0.3952</v>
+      </c>
+      <c r="E6">
+        <f>B6-0.134</f>
+        <v>0.313</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7">
+        <v>0.47299999999999998</v>
+      </c>
+      <c r="C7">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="D7">
+        <f>B7-0.00156</f>
+        <v>0.47143999999999997</v>
+      </c>
+      <c r="E7">
+        <f>B7-0.0272</f>
+        <v>0.44579999999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="C8">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="D8">
+        <f>B8-0.0181</f>
+        <v>0.2109</v>
+      </c>
+      <c r="E8">
+        <f>B8-0.065</f>
+        <v>0.16400000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>0.40400000000000003</v>
+      </c>
+      <c r="C9">
+        <v>5.96E-2</v>
+      </c>
+      <c r="D9">
+        <f>B9-0.0561</f>
+        <v>0.34790000000000004</v>
+      </c>
+      <c r="E9">
+        <f>B9-0.112</f>
+        <v>0.29200000000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7809DB9B-3FD8-5549-9FCD-267FEFC8FD9E}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -28643,7 +28686,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84F32D40-50E3-6642-8D70-05112DFB6AD6}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -28656,7 +28699,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41D1D4AF-07CA-6F49-AFFE-0C0473FEE9BF}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -28669,7 +28712,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5194872-4A7E-814B-947B-A32CCDF9E906}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -28682,7 +28725,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61859BC3-7413-7547-83A4-19282395964C}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>